<commit_message>
Model Noodling to match Jeff
</commit_message>
<xml_diff>
--- a/data/ModelResults.xlsx
+++ b/data/ModelResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/connerj_msu_edu/Documents/DocumentsOneDrive/Files/ConnerLabOneDrive/Arabidopsis/Stamen loss/European Population Surveys/Pyrenees/SophieAnalyses/R_script/StamenLossPipeline/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="8_{A5E90707-7E9A-4109-AE1B-D5AE205301FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F7AAC93-C19E-460B-99E4-ED3F3CB1E22E}"/>
+  <xr:revisionPtr revIDLastSave="197" documentId="8_{A5E90707-7E9A-4109-AE1B-D5AE205301FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{703A2206-1CBC-4BC3-A5A3-9EE5517CE342}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{E6D0F4C7-BFDF-463E-8B4C-67AB0A4A9DEB}"/>
   </bookViews>
@@ -40,15 +40,24 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={F9B97D6F-345D-42D3-9673-FF890F12A16B}</author>
+    <author>tc={41AD15BE-3653-419B-A96B-0DA140AFDBC0}</author>
   </authors>
   <commentList>
-    <comment ref="A32" authorId="0" shapeId="0" xr:uid="{F9B97D6F-345D-42D3-9673-FF890F12A16B}">
+    <comment ref="A44" authorId="0" shapeId="0" xr:uid="{F9B97D6F-345D-42D3-9673-FF890F12A16B}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Cent/nocent not important. This is only sequenced lines
 </t>
+      </text>
+    </comment>
+    <comment ref="A54" authorId="1" shapeId="0" xr:uid="{41AD15BE-3653-419B-A96B-0DA140AFDBC0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Cent/nocent not important. This is ALL lines</t>
       </text>
     </comment>
   </commentList>
@@ -74,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="49">
   <si>
     <t>Model</t>
   </si>
@@ -188,13 +197,46 @@
   </si>
   <si>
     <t>I did also fit this with no Elev_m2 but included an interaction term (Seq_PopFlwrmean ~ Elev_m * Mean.pi.c) - interaction was not significant</t>
+  </si>
+  <si>
+    <t>matches Jeff's mode</t>
+  </si>
+  <si>
+    <t>matches Jeff's model</t>
+  </si>
+  <si>
+    <t>DOES NOTE MATCH JEFF'S MODEL</t>
+  </si>
+  <si>
+    <t>( Elev_m - mean(Elev_m)^2</t>
+  </si>
+  <si>
+    <t>Full_PopFlwrMean ~ Elev_m +( Elev_m - mean(Elev_m)^2</t>
+  </si>
+  <si>
+    <t>matches Jeff's model; in R I calculate this first and call it Elev_c2</t>
+  </si>
+  <si>
+    <t>Full_PopFlwrMean ~ Elev_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full_PopFlwrMean ~ Elev_m </t>
+  </si>
+  <si>
+    <t>Full_PopFlwrMean ~ Elev_m + (Elev_m - mean(Elev_m))^2</t>
+  </si>
+  <si>
+    <t>or centered before squared</t>
+  </si>
+  <si>
+    <t>DOES NOT MATCH JEFF'S MODEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +251,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -237,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -245,23 +299,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{E3AD46BB-6877-4BB3-9366-22228BDB86FC}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -576,9 +658,12 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A32" dT="2023-08-07T17:27:10.83" personId="{0A4ED238-C52E-43C9-A873-668D7275502D}" id="{F9B97D6F-345D-42D3-9673-FF890F12A16B}">
+  <threadedComment ref="A44" dT="2023-08-07T17:27:10.83" personId="{0A4ED238-C52E-43C9-A873-668D7275502D}" id="{F9B97D6F-345D-42D3-9673-FF890F12A16B}">
     <text xml:space="preserve">Cent/nocent not important. This is only sequenced lines
 </text>
+  </threadedComment>
+  <threadedComment ref="A54" dT="2023-08-07T17:27:20.82" personId="{0A4ED238-C52E-43C9-A873-668D7275502D}" id="{41AD15BE-3653-419B-A96B-0DA140AFDBC0}">
+    <text>Cent/nocent not important. This is ALL lines</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -593,16 +678,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269D47F5-1F69-4D50-A220-50664C2E4743}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
@@ -610,753 +696,1176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="7">
         <v>1.1659999999999999E-3</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="8">
         <v>5.8299999999999998E-2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="7">
         <v>-3.0950000000000001E-7</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>0.32269999999999999</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="7">
         <v>155.1</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <v>0.15079999999999999</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="7">
         <v>0.49540000000000001</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="1">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7">
         <v>52.685499999999998</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="6">
         <v>0.379</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="6">
         <v>5.5730000000000002E-2</v>
       </c>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="7">
         <v>1.0510000000000001E-3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>0.1196</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="7">
         <v>-4.481E-7</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>0.20219999999999999</v>
       </c>
-      <c r="H5">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6">
         <v>0.25280000000000002</v>
       </c>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="7">
+        <v>3.8630000000000001E-4</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6">
+        <v>0.38190000000000002</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="7">
+        <v>4.8210000000000001E-4</v>
+      </c>
+      <c r="C7" s="10">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>-4.728E-7</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.137267</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6">
+        <v>0.48180000000000001</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B8" s="7">
         <v>2.5799999999999998E-4</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C8" s="11">
         <v>4.4103000000000003E-2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D8" s="7">
         <v>-4.728E-7</v>
       </c>
-      <c r="E6">
+      <c r="E8" s="6">
         <v>0.137267</v>
       </c>
-      <c r="H6">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6">
         <v>0.48180000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B9" s="7">
         <v>1.0859999999999999E-3</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C9" s="12">
         <v>8.5309999999999997E-2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D9" s="7">
         <v>-4.0649999999999999E-7</v>
       </c>
-      <c r="E7">
+      <c r="E9" s="6">
         <v>0.21005599999999999</v>
       </c>
-      <c r="H7">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6">
         <v>0.39639999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B10" s="7">
         <v>-1.672E-6</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C10" s="10">
         <v>1.8100000000000001E-4</v>
       </c>
-      <c r="H8">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6">
         <v>0.64459999999999995</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F9">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6">
         <v>-66.647099999999995</v>
       </c>
-      <c r="G9">
+      <c r="G11" s="6">
         <v>0.38700000000000001</v>
       </c>
-      <c r="H9">
+      <c r="H11" s="6">
         <v>5.3830000000000003E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="I11" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="1">
-        <v>52.685499999999998</v>
-      </c>
-      <c r="C13" s="1">
-        <v>57.960799999999999</v>
-      </c>
-      <c r="D13">
-        <v>0.90900000000000003</v>
-      </c>
-      <c r="E13">
-        <v>0.379</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>5.5730000000000002E-2</v>
+        <v>8</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.1659999999999999E-3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5.5730000000000005E-4</v>
+      </c>
+      <c r="D15">
+        <v>2.093</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5.8299999999999998E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>-1.172E-2</v>
+        <v>28</v>
+      </c>
+      <c r="B16" s="1">
+        <v>-3.0950000000000001E-7</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3.0009999999999999E-7</v>
+      </c>
+      <c r="D16">
+        <v>-1.0309999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.32269999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17">
-        <v>0.82630000000000003</v>
+        <v>34</v>
+      </c>
+      <c r="B17" s="1">
+        <v>155.1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>101.1</v>
+      </c>
+      <c r="D17">
+        <v>1.5349999999999999</v>
+      </c>
+      <c r="E17">
+        <v>0.15079999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>14</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.49540000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.36930000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3.9279999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B19">
-        <v>0.37869999999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="1">
+        <v>3.6400000000000002E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1.0510000000000001E-3</v>
-      </c>
-      <c r="C24" s="1">
-        <v>63100</v>
-      </c>
-      <c r="D24">
-        <v>1.6659999999999999</v>
-      </c>
-      <c r="E24">
-        <v>0.1196</v>
-      </c>
+      <c r="B24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="1">
-        <v>-4.481E-7</v>
-      </c>
-      <c r="C25" s="1">
-        <v>3.3360000000000002E-7</v>
-      </c>
-      <c r="D25">
-        <v>-1.343</v>
-      </c>
-      <c r="E25">
-        <v>0.20219999999999999</v>
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26">
-        <v>0.25280000000000002</v>
+        <v>34</v>
+      </c>
+      <c r="B26" s="1">
+        <v>52.685499999999998</v>
+      </c>
+      <c r="C26" s="1">
+        <v>57.960799999999999</v>
+      </c>
+      <c r="D26">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="E26">
+        <v>0.379</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27">
-        <v>0.13780000000000001</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B28">
-        <v>2.1989999999999998</v>
+        <v>5.5730000000000002E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B29">
-        <v>13</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
+        <v>-1.172E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>0.82630000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>24</v>
       </c>
-      <c r="B30">
+      <c r="B32">
+        <v>0.37869999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1.0510000000000001E-3</v>
+      </c>
+      <c r="C36" s="1">
+        <v>63100</v>
+      </c>
+      <c r="D36">
+        <v>1.6659999999999999</v>
+      </c>
+      <c r="E36">
+        <v>0.1196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="1">
+        <v>-4.481E-7</v>
+      </c>
+      <c r="C37" s="1">
+        <v>3.3360000000000002E-7</v>
+      </c>
+      <c r="D37">
+        <v>-1.343</v>
+      </c>
+      <c r="E37">
+        <v>0.20219999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>0.25280000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39">
+        <v>0.13780000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <v>2.1989999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42">
         <v>0.15049999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>2</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B45" t="s">
         <v>3</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C45" t="s">
         <v>4</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D45" t="s">
         <v>5</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E45" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B46" s="1">
         <v>1.0859999999999999E-3</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C46" s="1">
         <v>5.8299999999999997E-4</v>
       </c>
-      <c r="D34">
+      <c r="D46">
         <v>1.8620000000000001</v>
       </c>
-      <c r="E34">
+      <c r="E46">
         <v>8.5309999999999997E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B47" s="1">
         <v>-4.0649999999999999E-7</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C47" s="1">
         <v>3.0829999999999997E-7</v>
       </c>
-      <c r="D35">
+      <c r="D47">
         <v>-1.319</v>
       </c>
-      <c r="E35">
+      <c r="E47">
         <v>0.21005599999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>15</v>
-      </c>
-      <c r="B36">
-        <v>0.39639999999999997</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37">
-        <v>0.30349999999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38">
-        <v>4.2679999999999998</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-      <c r="C39">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40">
-        <v>3.7580000000000002E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="1">
-        <v>1.1659999999999999E-3</v>
-      </c>
-      <c r="C45" s="1">
-        <v>5.5730000000000005E-4</v>
-      </c>
-      <c r="D45">
-        <v>2.093</v>
-      </c>
-      <c r="E45" s="2">
-        <v>5.8299999999999998E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="1">
-        <v>-3.0950000000000001E-7</v>
-      </c>
-      <c r="C46" s="1">
-        <v>3.0009999999999999E-7</v>
-      </c>
-      <c r="D46">
-        <v>-1.0309999999999999</v>
-      </c>
-      <c r="E46">
-        <v>0.32269999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47" s="1">
-        <v>155.1</v>
-      </c>
-      <c r="C47" s="1">
-        <v>101.1</v>
-      </c>
-      <c r="D47">
-        <v>1.5349999999999999</v>
-      </c>
-      <c r="E47">
-        <v>0.15079999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="1">
-        <v>0.49540000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>0.39639999999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="1">
-        <v>0.36930000000000002</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>0.30349999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>20</v>
       </c>
-      <c r="B50" s="1">
-        <v>3.9279999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>4.2679999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="1">
-        <v>3</v>
+      <c r="B51">
+        <v>2</v>
       </c>
       <c r="C51">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
-      <c r="B52" s="1">
-        <v>3.6400000000000002E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="B52">
+        <v>3.7580000000000002E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B54" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1.2600000000000001E-3</v>
+      </c>
+      <c r="C56" s="1">
+        <v>5.6459999999999995E-4</v>
+      </c>
+      <c r="D56">
+        <v>2.2290000000000001</v>
+      </c>
+      <c r="E56">
+        <v>4.4103000000000003E-2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" s="1">
+        <v>-4.728E-7</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2.9849999999999998E-7</v>
+      </c>
+      <c r="D57">
+        <v>-1.5840000000000001</v>
+      </c>
+      <c r="E57">
+        <v>0.137267</v>
+      </c>
+      <c r="F57" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58">
+        <v>0.48180000000000001</v>
+      </c>
+      <c r="F58" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59">
+        <v>0.40210000000000001</v>
+      </c>
+      <c r="F59" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60">
+        <v>6.0449999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>13</v>
+      </c>
+      <c r="F61" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62">
+        <v>1.393E-2</v>
+      </c>
+      <c r="F62" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="3">
+        <v>4.8210000000000001E-4</v>
+      </c>
+      <c r="C66" s="3">
+        <v>1.3870000000000001E-4</v>
+      </c>
+      <c r="D66" s="4">
+        <v>3.476</v>
+      </c>
+      <c r="E66" s="4">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="F66" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>41</v>
+      </c>
+      <c r="B67" s="3">
+        <v>-4.728E-7</v>
+      </c>
+      <c r="C67" s="3">
+        <v>2.9849999999999998E-7</v>
+      </c>
+      <c r="D67" s="4">
+        <v>-1.5840000000000001</v>
+      </c>
+      <c r="E67" s="4">
+        <v>0.13730000000000001</v>
+      </c>
+      <c r="F67" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68">
+        <v>0.48180000000000001</v>
+      </c>
+      <c r="F68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69">
+        <v>0.40210000000000001</v>
+      </c>
+      <c r="F69" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70">
+        <v>6.0449999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71">
+        <v>13</v>
+      </c>
+      <c r="F71" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72">
+        <v>1.393E-2</v>
+      </c>
+      <c r="F72" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="4">
+        <v>3.8630000000000001E-4</v>
+      </c>
+      <c r="C76" s="4">
+        <v>1.314E-4</v>
+      </c>
+      <c r="D76" s="4">
+        <v>2.9409999999999998</v>
+      </c>
+      <c r="E76" s="4">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="F76" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>15</v>
+      </c>
+      <c r="B77" s="4">
+        <v>0.38190000000000002</v>
+      </c>
+      <c r="F77" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78" s="4">
+        <v>0.3377</v>
+      </c>
+      <c r="F78" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" s="4">
+        <v>8.6489999999999991</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>14</v>
+      </c>
+      <c r="F80" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="4">
+        <v>1.074E-2</v>
+      </c>
+      <c r="F81" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>2</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B84" t="s">
         <v>3</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C84" t="s">
         <v>4</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D84" t="s">
         <v>5</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E84" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>8</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B85" s="1">
         <v>-1.672E-6</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C85" s="1">
         <v>3.3169999999999999E-7</v>
       </c>
-      <c r="D57">
+      <c r="D85">
         <v>-5.0389999999999997</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E85" s="2">
         <v>1.8100000000000001E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>15</v>
       </c>
-      <c r="B59">
+      <c r="B87">
         <v>0.64459999999999995</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>18</v>
       </c>
-      <c r="B60">
+      <c r="B88">
         <v>0.61929999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>20</v>
       </c>
-      <c r="B61">
+      <c r="B89">
         <v>25.4</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>22</v>
       </c>
-      <c r="B62">
+      <c r="B90">
         <v>14</v>
       </c>
-      <c r="C62">
+      <c r="C90">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>24</v>
       </c>
-      <c r="B63">
+      <c r="B91">
         <v>1.808E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>2</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B95" t="s">
         <v>3</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C95" t="s">
         <v>4</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D95" t="s">
         <v>5</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E95" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>27</v>
       </c>
-      <c r="B68">
+      <c r="B96">
         <v>-66.647099999999995</v>
       </c>
-      <c r="C68">
+      <c r="C96">
         <v>74.677700000000002</v>
       </c>
-      <c r="D68">
+      <c r="D96">
         <v>-0.89200000000000002</v>
       </c>
-      <c r="E68">
+      <c r="E96">
         <v>0.38700000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>15</v>
       </c>
-      <c r="B70">
+      <c r="B98">
         <v>5.3830000000000003E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>18</v>
       </c>
-      <c r="B71">
+      <c r="B99">
         <v>-1.375E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>20</v>
       </c>
-      <c r="B72">
+      <c r="B100">
         <v>0.79649999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>22</v>
       </c>
-      <c r="B73">
+      <c r="B101">
         <v>14</v>
       </c>
-      <c r="C73">
+      <c r="C101">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>24</v>
       </c>
-      <c r="B74">
+      <c r="B102">
         <v>0.38719999999999999</v>
       </c>
     </row>
@@ -1372,11 +1881,13 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="47" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
@@ -1628,7 +2139,7 @@
         <v>5.398E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1636,7 +2147,7 @@
         <v>-1.359E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1644,7 +2155,7 @@
         <v>0.79879999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1655,7 +2166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1663,7 +2174,7 @@
         <v>0.38650000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -1671,7 +2182,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1688,12 +2199,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="1">
-        <v>2.5799999999999998E-4</v>
+        <v>1.2600000000000001E-3</v>
       </c>
       <c r="C24" s="1">
         <v>5.6459999999999995E-4</v>
@@ -1704,8 +2215,11 @@
       <c r="E24">
         <v>4.4103000000000003E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1721,24 +2235,33 @@
       <c r="E25">
         <v>0.137267</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
       <c r="B26">
         <v>0.48180000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
       <c r="B27">
         <v>0.40210000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1746,7 +2269,7 @@
         <v>6.0449999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1756,13 +2279,19 @@
       <c r="C29">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
       <c r="B30">
         <v>1.393E-2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to Centered Quadratic
</commit_message>
<xml_diff>
--- a/data/ModelResults.xlsx
+++ b/data/ModelResults.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/connerj_msu_edu/Documents/DocumentsOneDrive/Files/ConnerLabOneDrive/Arabidopsis/Stamen loss/European Population Surveys/Pyrenees/SophieAnalyses/R_script/StamenLossPipeline/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="8_{A5E90707-7E9A-4109-AE1B-D5AE205301FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{703A2206-1CBC-4BC3-A5A3-9EE5517CE342}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="8_{A5E90707-7E9A-4109-AE1B-D5AE205301FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{254F719E-8A93-46DE-9846-40C1628E60C4}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{E6D0F4C7-BFDF-463E-8B4C-67AB0A4A9DEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="NoCent" sheetId="2" r:id="rId1"/>
-    <sheet name="Cent" sheetId="1" r:id="rId2"/>
+    <sheet name="Cent" sheetId="1" r:id="rId1"/>
+    <sheet name="NoCent" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,6 +37,34 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={03716D33-722B-430E-A1DB-B756141A1E58}</author>
+    <author>tc={40587295-A488-494D-94F6-449F92B50906}</author>
+  </authors>
+  <commentList>
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{03716D33-722B-430E-A1DB-B756141A1E58}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is sometimes centered depending on the model
+</t>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="1" shapeId="0" xr:uid="{40587295-A488-494D-94F6-449F92B50906}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Cent/nocent not important. This is ALL lines</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={F9B97D6F-345D-42D3-9673-FF890F12A16B}</author>
@@ -64,26 +92,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={40587295-A488-494D-94F6-449F92B50906}</author>
-  </authors>
-  <commentList>
-    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{40587295-A488-494D-94F6-449F92B50906}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Cent/nocent not important. This is ALL lines</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="58">
   <si>
     <t>Model</t>
   </si>
@@ -133,9 +143,6 @@
     <t>r2</t>
   </si>
   <si>
-    <t>Seq_PopFlwrMean ~ Elev_m _ Elev_m2 + mean.pi</t>
-  </si>
-  <si>
     <t>Elev_residuals ~ mean.pi</t>
   </si>
   <si>
@@ -230,6 +237,36 @@
   </si>
   <si>
     <t>DOES NOT MATCH JEFF'S MODEL</t>
+  </si>
+  <si>
+    <t>Seq_PopFlwrMean ~ Elev_m + Elev_c2 + Mean.pi</t>
+  </si>
+  <si>
+    <t>Elev_c2 is the centered quadratic terms.</t>
+  </si>
+  <si>
+    <t>Seq_PopFlwrMean ~ Elev_m _ Elev_c2 + mean.pi</t>
+  </si>
+  <si>
+    <t>this one is centered quadratic still!</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Seq_PopFlwrMean ~ Elev_m + (Elev_m - mean(Elev_m))^2</t>
+  </si>
+  <si>
+    <t>no full details; residuals of this model used for resid(elev) ~ pi</t>
+  </si>
+  <si>
+    <t>PI_residuals ~ Elev_m _ Elev_c2</t>
+  </si>
+  <si>
+    <t>Pi_residuals ~ Elev_m + Elev_c2</t>
+  </si>
+  <si>
+    <t>Elev_c2</t>
   </si>
 </sst>
 </file>
@@ -318,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -336,6 +373,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,6 +696,18 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="L3" dT="2023-10-26T20:29:24.10" personId="{0A4ED238-C52E-43C9-A873-668D7275502D}" id="{03716D33-722B-430E-A1DB-B756141A1E58}">
+    <text xml:space="preserve">This is sometimes centered depending on the model
+</text>
+  </threadedComment>
+  <threadedComment ref="A22" dT="2023-08-07T17:27:20.82" personId="{0A4ED238-C52E-43C9-A873-668D7275502D}" id="{40587295-A488-494D-94F6-449F92B50906}">
+    <text>Cent/nocent not important. This is ALL lines</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A44" dT="2023-08-07T17:27:10.83" personId="{0A4ED238-C52E-43C9-A873-668D7275502D}" id="{F9B97D6F-345D-42D3-9673-FF890F12A16B}">
     <text xml:space="preserve">Cent/nocent not important. This is only sequenced lines
 </text>
@@ -668,20 +718,839 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A22" dT="2023-08-07T17:27:20.82" personId="{0A4ED238-C52E-43C9-A873-668D7275502D}" id="{40587295-A488-494D-94F6-449F92B50906}">
-    <text>Cent/nocent not important. This is ALL lines</text>
-  </threadedComment>
-</ThreadedComments>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC43E702-708E-4929-83A6-563C048BC86A}">
+  <dimension ref="A1:Q60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-1.8059999999999999E-6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3.6119999999999998E-7</v>
+      </c>
+      <c r="D3">
+        <v>-5.0010000000000003</v>
+      </c>
+      <c r="E3">
+        <v>1.94E-4</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="1">
+        <v>6.4670000000000005E-4</v>
+      </c>
+      <c r="K4">
+        <v>8.8199999999999997E-3</v>
+      </c>
+      <c r="L4" s="1">
+        <v>-2.9900000000000002E-7</v>
+      </c>
+      <c r="M4">
+        <v>0.34514</v>
+      </c>
+      <c r="N4" s="1">
+        <v>138.5</v>
+      </c>
+      <c r="O4">
+        <v>0.16696</v>
+      </c>
+      <c r="P4">
+        <v>0.48859999999999998</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0.6411</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="1">
+        <v>46.827800000000003</v>
+      </c>
+      <c r="O5">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="P5">
+        <v>5.1679999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>0.61550000000000005</v>
+      </c>
+      <c r="I6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="3">
+        <v>3.1690000000000001E-4</v>
+      </c>
+      <c r="K6">
+        <v>3.1600000000000003E-2</v>
+      </c>
+      <c r="L6" s="3">
+        <v>-4.5429999999999999E-7</v>
+      </c>
+      <c r="M6">
+        <v>0.19550000000000001</v>
+      </c>
+      <c r="P6">
+        <v>0.25590000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>25.01</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="7">
+        <v>4.8210000000000001E-4</v>
+      </c>
+      <c r="K7" s="10">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="L7" s="7">
+        <v>-4.728E-7</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0.137267</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6">
+        <v>0.48180000000000001</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2.5799999999999998E-4</v>
+      </c>
+      <c r="K8">
+        <v>4.4103000000000003E-2</v>
+      </c>
+      <c r="L8" s="1">
+        <v>-4.728E-7</v>
+      </c>
+      <c r="M8">
+        <v>0.137267</v>
+      </c>
+      <c r="P8">
+        <v>0.48180000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>1.942E-4</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="1">
+        <v>4.1839999999999998E-4</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="L9" s="1">
+        <v>-4.0649999999999999E-7</v>
+      </c>
+      <c r="M9" s="13">
+        <v>0.21010000000000001</v>
+      </c>
+      <c r="P9">
+        <v>0.39639999999999997</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.0859999999999999E-3</v>
+      </c>
+      <c r="K10">
+        <v>8.5309999999999997E-2</v>
+      </c>
+      <c r="L10" s="1">
+        <v>-4.0649999999999999E-7</v>
+      </c>
+      <c r="M10">
+        <v>0.21005599999999999</v>
+      </c>
+      <c r="P10">
+        <v>0.39639999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-1.8059999999999999E-6</v>
+      </c>
+      <c r="K11">
+        <v>1.94E-4</v>
+      </c>
+      <c r="P11">
+        <v>0.6411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12">
+        <v>-61.598500000000001</v>
+      </c>
+      <c r="O12">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="P12">
+        <v>5.398E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>-61.598500000000001</v>
+      </c>
+      <c r="C14">
+        <v>68.919200000000004</v>
+      </c>
+      <c r="D14">
+        <v>-0.89400000000000002</v>
+      </c>
+      <c r="E14">
+        <v>0.38700000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>5.398E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>-1.359E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>0.79879999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>0.38650000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.2600000000000001E-3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5.6459999999999995E-4</v>
+      </c>
+      <c r="D24">
+        <v>2.2290000000000001</v>
+      </c>
+      <c r="E24">
+        <v>4.4103000000000003E-2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1">
+        <v>-4.728E-7</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2.9849999999999998E-7</v>
+      </c>
+      <c r="D25">
+        <v>-1.5840000000000001</v>
+      </c>
+      <c r="E25">
+        <v>0.137267</v>
+      </c>
+      <c r="F25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>0.48180000000000001</v>
+      </c>
+      <c r="F26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>0.40210000000000001</v>
+      </c>
+      <c r="F27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28">
+        <v>6.0449999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <v>1.393E-2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1">
+        <v>6.4670000000000005E-4</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2.0709999999999999E-4</v>
+      </c>
+      <c r="D34">
+        <v>3.1219999999999999</v>
+      </c>
+      <c r="E34">
+        <v>8.8199999999999997E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-2.9900000000000002E-7</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3.0419999999999998E-7</v>
+      </c>
+      <c r="D35">
+        <v>-0.98299999999999998</v>
+      </c>
+      <c r="E35">
+        <v>0.34514</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="1">
+        <v>138.5</v>
+      </c>
+      <c r="C36" s="1">
+        <v>94.11</v>
+      </c>
+      <c r="D36">
+        <v>1.4710000000000001</v>
+      </c>
+      <c r="E36">
+        <v>0.16696</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.48859999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.36080000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3.8220000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="1">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="1">
+        <v>3.9239999999999997E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="1">
+        <v>46.827800000000003</v>
+      </c>
+      <c r="C45" s="1">
+        <v>53.610100000000003</v>
+      </c>
+      <c r="D45">
+        <v>0.873</v>
+      </c>
+      <c r="E45">
+        <v>0.39700000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="1">
+        <v>5.1679999999999997E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="1">
+        <v>-1.6049999999999998E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.39710000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="3">
+        <v>3.1690000000000001E-4</v>
+      </c>
+      <c r="C54" s="3">
+        <v>1.5469999999999999E-4</v>
+      </c>
+      <c r="D54">
+        <v>2.0489999999999999</v>
+      </c>
+      <c r="E54">
+        <v>6.13E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="3">
+        <v>-4.5429999999999999E-7</v>
+      </c>
+      <c r="C55" s="3">
+        <v>3.3290000000000002E-7</v>
+      </c>
+      <c r="D55">
+        <v>-1.365</v>
+      </c>
+      <c r="E55">
+        <v>0.19550000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0.25590000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0.1414</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2.2349999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0.1464</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269D47F5-1F69-4D50-A220-50664C2E4743}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +1571,7 @@
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -736,12 +1605,12 @@
         <v>15</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="7">
         <v>1.1659999999999999E-3</v>
@@ -765,12 +1634,12 @@
         <v>0.49540000000000001</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -789,7 +1658,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="7">
         <v>1.0510000000000001E-3</v>
@@ -812,7 +1681,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="7">
         <v>3.8630000000000001E-4</v>
@@ -828,12 +1697,12 @@
         <v>0.38190000000000002</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="7">
         <v>4.8210000000000001E-4</v>
@@ -853,12 +1722,12 @@
         <v>0.48180000000000001</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="7">
         <v>2.5799999999999998E-4</v>
@@ -881,7 +1750,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="7">
         <v>1.0859999999999999E-3</v>
@@ -904,7 +1773,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="7">
         <v>-1.672E-6</v>
@@ -923,7 +1792,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -945,10 +1814,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -987,7 +1856,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1">
         <v>-3.0950000000000001E-7</v>
@@ -1004,7 +1873,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1">
         <v>155.1</v>
@@ -1029,7 +1898,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>0.36930000000000002</v>
@@ -1037,7 +1906,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>3.9279999999999999</v>
@@ -1045,7 +1914,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>3</v>
@@ -1056,7 +1925,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1">
         <v>3.6400000000000002E-2</v>
@@ -1070,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="2"/>
     </row>
@@ -1093,7 +1962,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1">
         <v>52.685499999999998</v>
@@ -1122,7 +1991,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29">
         <v>-1.172E-2</v>
@@ -1130,7 +1999,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30">
         <v>0.82630000000000003</v>
@@ -1138,7 +2007,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1149,7 +2018,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32">
         <v>0.37869999999999998</v>
@@ -1160,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1199,7 +2068,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1">
         <v>-4.481E-7</v>
@@ -1224,7 +2093,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39">
         <v>0.13780000000000001</v>
@@ -1232,7 +2101,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40">
         <v>2.1989999999999998</v>
@@ -1240,7 +2109,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -1251,7 +2120,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B42">
         <v>0.15049999999999999</v>
@@ -1262,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1301,7 +2170,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B47" s="1">
         <v>-4.0649999999999999E-7</v>
@@ -1326,7 +2195,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B49">
         <v>0.30349999999999999</v>
@@ -1334,7 +2203,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50">
         <v>4.2679999999999998</v>
@@ -1342,7 +2211,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -1353,7 +2222,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B52">
         <v>3.7580000000000002E-2</v>
@@ -1364,7 +2233,7 @@
         <v>0</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1401,12 +2270,12 @@
         <v>4.4103000000000003E-2</v>
       </c>
       <c r="F56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B57" s="1">
         <v>-4.728E-7</v>
@@ -1421,7 +2290,7 @@
         <v>0.137267</v>
       </c>
       <c r="F57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1432,23 +2301,23 @@
         <v>0.48180000000000001</v>
       </c>
       <c r="F58" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B59">
         <v>0.40210000000000001</v>
       </c>
       <c r="F59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B60">
         <v>6.0449999999999999</v>
@@ -1456,7 +2325,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -1465,18 +2334,18 @@
         <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B62">
         <v>1.393E-2</v>
       </c>
       <c r="F62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1484,7 +2353,7 @@
         <v>0</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1521,12 +2390,12 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="F66" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B67" s="3">
         <v>-4.728E-7</v>
@@ -1541,7 +2410,7 @@
         <v>0.13730000000000001</v>
       </c>
       <c r="F67" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1552,23 +2421,23 @@
         <v>0.48180000000000001</v>
       </c>
       <c r="F68" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B69">
         <v>0.40210000000000001</v>
       </c>
       <c r="F69" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B70">
         <v>6.0449999999999999</v>
@@ -1576,7 +2445,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B71">
         <v>2</v>
@@ -1585,18 +2454,18 @@
         <v>13</v>
       </c>
       <c r="F71" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B72">
         <v>1.393E-2</v>
       </c>
       <c r="F72" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1604,7 +2473,7 @@
         <v>0</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -1641,7 +2510,7 @@
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="F76" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -1652,23 +2521,23 @@
         <v>0.38190000000000002</v>
       </c>
       <c r="F77" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B78" s="4">
         <v>0.3377</v>
       </c>
       <c r="F78" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B79" s="4">
         <v>8.6489999999999991</v>
@@ -1676,7 +2545,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -1685,18 +2554,18 @@
         <v>14</v>
       </c>
       <c r="F80" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B81" s="4">
         <v>1.074E-2</v>
       </c>
       <c r="F81" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -1704,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -1751,7 +2620,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B88">
         <v>0.61929999999999996</v>
@@ -1759,7 +2628,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B89">
         <v>25.4</v>
@@ -1767,7 +2636,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B90">
         <v>14</v>
@@ -1778,7 +2647,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B91">
         <v>1.808E-4</v>
@@ -1789,7 +2658,7 @@
         <v>0</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -1811,7 +2680,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B96">
         <v>-66.647099999999995</v>
@@ -1836,7 +2705,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B99">
         <v>-1.375E-2</v>
@@ -1844,7 +2713,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B100">
         <v>0.79649999999999999</v>
@@ -1852,7 +2721,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B101">
         <v>14</v>
@@ -1863,7 +2732,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B102">
         <v>0.38719999999999999</v>
@@ -1874,428 +2743,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC43E702-708E-4929-83A6-563C048BC86A}">
-  <dimension ref="A1:P30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1">
-        <v>-1.8059999999999999E-6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3.6119999999999998E-7</v>
-      </c>
-      <c r="D3">
-        <v>-5.0010000000000003</v>
-      </c>
-      <c r="E3">
-        <v>1.94E-4</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>0.6411</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>0.61550000000000005</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7">
-        <v>25.01</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="1">
-        <v>2.5799999999999998E-4</v>
-      </c>
-      <c r="K7">
-        <v>4.4103000000000003E-2</v>
-      </c>
-      <c r="L7" s="1">
-        <v>-4.728E-7</v>
-      </c>
-      <c r="M7">
-        <v>0.137267</v>
-      </c>
-      <c r="P7">
-        <v>0.48180000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1.0859999999999999E-3</v>
-      </c>
-      <c r="K8">
-        <v>8.5309999999999997E-2</v>
-      </c>
-      <c r="L8" s="1">
-        <v>-4.0649999999999999E-7</v>
-      </c>
-      <c r="M8">
-        <v>0.21005599999999999</v>
-      </c>
-      <c r="P8">
-        <v>0.39639999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9">
-        <v>1.942E-4</v>
-      </c>
-      <c r="I9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="1">
-        <v>-1.8059999999999999E-6</v>
-      </c>
-      <c r="K9">
-        <v>1.94E-4</v>
-      </c>
-      <c r="P9">
-        <v>0.6411</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N10">
-        <v>-61.598500000000001</v>
-      </c>
-      <c r="O10">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="P10">
-        <v>5.398E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14">
-        <v>-61.598500000000001</v>
-      </c>
-      <c r="C14">
-        <v>68.919200000000004</v>
-      </c>
-      <c r="D14">
-        <v>-0.89400000000000002</v>
-      </c>
-      <c r="E14">
-        <v>0.38700000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>5.398E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>-1.359E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>0.79879999999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19">
-        <v>14</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20">
-        <v>0.38650000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1.2600000000000001E-3</v>
-      </c>
-      <c r="C24" s="1">
-        <v>5.6459999999999995E-4</v>
-      </c>
-      <c r="D24">
-        <v>2.2290000000000001</v>
-      </c>
-      <c r="E24">
-        <v>4.4103000000000003E-2</v>
-      </c>
-      <c r="F24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="1">
-        <v>-4.728E-7</v>
-      </c>
-      <c r="C25" s="1">
-        <v>2.9849999999999998E-7</v>
-      </c>
-      <c r="D25">
-        <v>-1.5840000000000001</v>
-      </c>
-      <c r="E25">
-        <v>0.137267</v>
-      </c>
-      <c r="F25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26">
-        <v>0.48180000000000001</v>
-      </c>
-      <c r="F26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27">
-        <v>0.40210000000000001</v>
-      </c>
-      <c r="F27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28">
-        <v>6.0449999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="C29">
-        <v>13</v>
-      </c>
-      <c r="F29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30">
-        <v>1.393E-2</v>
-      </c>
-      <c r="F30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Clean Files, updates GWAS figures
</commit_message>
<xml_diff>
--- a/data/ModelResults.xlsx
+++ b/data/ModelResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/connerj_msu_edu/Documents/DocumentsOneDrive/Files/ConnerLabOneDrive/Arabidopsis/Stamen loss/European Population Surveys/Pyrenees/SophieAnalyses/R_script/StamenLossPipeline/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="380" documentId="8_{A5E90707-7E9A-4109-AE1B-D5AE205301FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD467C65-92A3-4C97-9916-A8DEDCBE87DD}"/>
+  <xr:revisionPtr revIDLastSave="391" documentId="8_{A5E90707-7E9A-4109-AE1B-D5AE205301FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5918F73B-F11E-4A76-B4F3-BC41C6FD4D17}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6D0F4C7-BFDF-463E-8B4C-67AB0A4A9DEB}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{E6D0F4C7-BFDF-463E-8B4C-67AB0A4A9DEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Formatted" sheetId="3" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="75">
   <si>
     <t>Model</t>
   </si>
@@ -303,22 +303,6 @@
   <si>
     <r>
       <t>Full_PopFlwrMean ~ Elevation + (centered Elevation)</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Seq_PopFlwrMean ~Elevation + (centered Elevation)</t>
     </r>
     <r>
       <rPr>
@@ -424,6 +408,25 @@
   </si>
   <si>
     <t>Nucleotide Diversity p value</t>
+  </si>
+  <si>
+    <r>
+      <t>Seq_PopFlwrMean ~ Elevation + (centered Elevation)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Nucleotide Diversity ~ Elevation</t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -578,6 +581,8 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -587,10 +592,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D38E34F-ADC0-4713-B33F-86E3FA4A121C}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:XEX9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,42 +957,42 @@
     <col min="9" max="9" width="47.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>15</v>
@@ -1000,143 +1001,2211 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="7">
+        <v>-1.8059999999999999E-6</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1.94E-4</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="6">
+        <v>0.6411</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AX3" s="1"/>
+      <c r="BF3" s="1"/>
+      <c r="BN3" s="1"/>
+      <c r="BV3" s="1"/>
+      <c r="CD3" s="1"/>
+      <c r="CL3" s="1"/>
+      <c r="CT3" s="1"/>
+      <c r="DB3" s="1"/>
+      <c r="DJ3" s="1"/>
+      <c r="DR3" s="1"/>
+      <c r="DZ3" s="1"/>
+      <c r="EH3" s="1"/>
+      <c r="EP3" s="1"/>
+      <c r="EX3" s="1"/>
+      <c r="FF3" s="1"/>
+      <c r="FN3" s="1"/>
+      <c r="FV3" s="1"/>
+      <c r="GD3" s="1"/>
+      <c r="GL3" s="1"/>
+      <c r="GT3" s="1"/>
+      <c r="HB3" s="1"/>
+      <c r="HJ3" s="1"/>
+      <c r="HR3" s="1"/>
+      <c r="HZ3" s="1"/>
+      <c r="IH3" s="1"/>
+      <c r="IP3" s="1"/>
+      <c r="IX3" s="1"/>
+      <c r="JF3" s="1"/>
+      <c r="JN3" s="1"/>
+      <c r="JV3" s="1"/>
+      <c r="KD3" s="1"/>
+      <c r="KL3" s="1"/>
+      <c r="KT3" s="1"/>
+      <c r="LB3" s="1"/>
+      <c r="LJ3" s="1"/>
+      <c r="LR3" s="1"/>
+      <c r="LZ3" s="1"/>
+      <c r="MH3" s="1"/>
+      <c r="MP3" s="1"/>
+      <c r="MX3" s="1"/>
+      <c r="NF3" s="1"/>
+      <c r="NN3" s="1"/>
+      <c r="NV3" s="1"/>
+      <c r="OD3" s="1"/>
+      <c r="OL3" s="1"/>
+      <c r="OT3" s="1"/>
+      <c r="PB3" s="1"/>
+      <c r="PJ3" s="1"/>
+      <c r="PR3" s="1"/>
+      <c r="PZ3" s="1"/>
+      <c r="QH3" s="1"/>
+      <c r="QP3" s="1"/>
+      <c r="QX3" s="1"/>
+      <c r="RF3" s="1"/>
+      <c r="RN3" s="1"/>
+      <c r="RV3" s="1"/>
+      <c r="SD3" s="1"/>
+      <c r="SL3" s="1"/>
+      <c r="ST3" s="1"/>
+      <c r="TB3" s="1"/>
+      <c r="TJ3" s="1"/>
+      <c r="TR3" s="1"/>
+      <c r="TZ3" s="1"/>
+      <c r="UH3" s="1"/>
+      <c r="UP3" s="1"/>
+      <c r="UX3" s="1"/>
+      <c r="VF3" s="1"/>
+      <c r="VN3" s="1"/>
+      <c r="VV3" s="1"/>
+      <c r="WD3" s="1"/>
+      <c r="WL3" s="1"/>
+      <c r="WT3" s="1"/>
+      <c r="XB3" s="1"/>
+      <c r="XJ3" s="1"/>
+      <c r="XR3" s="1"/>
+      <c r="XZ3" s="1"/>
+      <c r="YH3" s="1"/>
+      <c r="YP3" s="1"/>
+      <c r="YX3" s="1"/>
+      <c r="ZF3" s="1"/>
+      <c r="ZN3" s="1"/>
+      <c r="ZV3" s="1"/>
+      <c r="AAD3" s="1"/>
+      <c r="AAL3" s="1"/>
+      <c r="AAT3" s="1"/>
+      <c r="ABB3" s="1"/>
+      <c r="ABJ3" s="1"/>
+      <c r="ABR3" s="1"/>
+      <c r="ABZ3" s="1"/>
+      <c r="ACH3" s="1"/>
+      <c r="ACP3" s="1"/>
+      <c r="ACX3" s="1"/>
+      <c r="ADF3" s="1"/>
+      <c r="ADN3" s="1"/>
+      <c r="ADV3" s="1"/>
+      <c r="AED3" s="1"/>
+      <c r="AEL3" s="1"/>
+      <c r="AET3" s="1"/>
+      <c r="AFB3" s="1"/>
+      <c r="AFJ3" s="1"/>
+      <c r="AFR3" s="1"/>
+      <c r="AFZ3" s="1"/>
+      <c r="AGH3" s="1"/>
+      <c r="AGP3" s="1"/>
+      <c r="AGX3" s="1"/>
+      <c r="AHF3" s="1"/>
+      <c r="AHN3" s="1"/>
+      <c r="AHV3" s="1"/>
+      <c r="AID3" s="1"/>
+      <c r="AIL3" s="1"/>
+      <c r="AIT3" s="1"/>
+      <c r="AJB3" s="1"/>
+      <c r="AJJ3" s="1"/>
+      <c r="AJR3" s="1"/>
+      <c r="AJZ3" s="1"/>
+      <c r="AKH3" s="1"/>
+      <c r="AKP3" s="1"/>
+      <c r="AKX3" s="1"/>
+      <c r="ALF3" s="1"/>
+      <c r="ALN3" s="1"/>
+      <c r="ALV3" s="1"/>
+      <c r="AMD3" s="1"/>
+      <c r="AML3" s="1"/>
+      <c r="AMT3" s="1"/>
+      <c r="ANB3" s="1"/>
+      <c r="ANJ3" s="1"/>
+      <c r="ANR3" s="1"/>
+      <c r="ANZ3" s="1"/>
+      <c r="AOH3" s="1"/>
+      <c r="AOP3" s="1"/>
+      <c r="AOX3" s="1"/>
+      <c r="APF3" s="1"/>
+      <c r="APN3" s="1"/>
+      <c r="APV3" s="1"/>
+      <c r="AQD3" s="1"/>
+      <c r="AQL3" s="1"/>
+      <c r="AQT3" s="1"/>
+      <c r="ARB3" s="1"/>
+      <c r="ARJ3" s="1"/>
+      <c r="ARR3" s="1"/>
+      <c r="ARZ3" s="1"/>
+      <c r="ASH3" s="1"/>
+      <c r="ASP3" s="1"/>
+      <c r="ASX3" s="1"/>
+      <c r="ATF3" s="1"/>
+      <c r="ATN3" s="1"/>
+      <c r="ATV3" s="1"/>
+      <c r="AUD3" s="1"/>
+      <c r="AUL3" s="1"/>
+      <c r="AUT3" s="1"/>
+      <c r="AVB3" s="1"/>
+      <c r="AVJ3" s="1"/>
+      <c r="AVR3" s="1"/>
+      <c r="AVZ3" s="1"/>
+      <c r="AWH3" s="1"/>
+      <c r="AWP3" s="1"/>
+      <c r="AWX3" s="1"/>
+      <c r="AXF3" s="1"/>
+      <c r="AXN3" s="1"/>
+      <c r="AXV3" s="1"/>
+      <c r="AYD3" s="1"/>
+      <c r="AYL3" s="1"/>
+      <c r="AYT3" s="1"/>
+      <c r="AZB3" s="1"/>
+      <c r="AZJ3" s="1"/>
+      <c r="AZR3" s="1"/>
+      <c r="AZZ3" s="1"/>
+      <c r="BAH3" s="1"/>
+      <c r="BAP3" s="1"/>
+      <c r="BAX3" s="1"/>
+      <c r="BBF3" s="1"/>
+      <c r="BBN3" s="1"/>
+      <c r="BBV3" s="1"/>
+      <c r="BCD3" s="1"/>
+      <c r="BCL3" s="1"/>
+      <c r="BCT3" s="1"/>
+      <c r="BDB3" s="1"/>
+      <c r="BDJ3" s="1"/>
+      <c r="BDR3" s="1"/>
+      <c r="BDZ3" s="1"/>
+      <c r="BEH3" s="1"/>
+      <c r="BEP3" s="1"/>
+      <c r="BEX3" s="1"/>
+      <c r="BFF3" s="1"/>
+      <c r="BFN3" s="1"/>
+      <c r="BFV3" s="1"/>
+      <c r="BGD3" s="1"/>
+      <c r="BGL3" s="1"/>
+      <c r="BGT3" s="1"/>
+      <c r="BHB3" s="1"/>
+      <c r="BHJ3" s="1"/>
+      <c r="BHR3" s="1"/>
+      <c r="BHZ3" s="1"/>
+      <c r="BIH3" s="1"/>
+      <c r="BIP3" s="1"/>
+      <c r="BIX3" s="1"/>
+      <c r="BJF3" s="1"/>
+      <c r="BJN3" s="1"/>
+      <c r="BJV3" s="1"/>
+      <c r="BKD3" s="1"/>
+      <c r="BKL3" s="1"/>
+      <c r="BKT3" s="1"/>
+      <c r="BLB3" s="1"/>
+      <c r="BLJ3" s="1"/>
+      <c r="BLR3" s="1"/>
+      <c r="BLZ3" s="1"/>
+      <c r="BMH3" s="1"/>
+      <c r="BMP3" s="1"/>
+      <c r="BMX3" s="1"/>
+      <c r="BNF3" s="1"/>
+      <c r="BNN3" s="1"/>
+      <c r="BNV3" s="1"/>
+      <c r="BOD3" s="1"/>
+      <c r="BOL3" s="1"/>
+      <c r="BOT3" s="1"/>
+      <c r="BPB3" s="1"/>
+      <c r="BPJ3" s="1"/>
+      <c r="BPR3" s="1"/>
+      <c r="BPZ3" s="1"/>
+      <c r="BQH3" s="1"/>
+      <c r="BQP3" s="1"/>
+      <c r="BQX3" s="1"/>
+      <c r="BRF3" s="1"/>
+      <c r="BRN3" s="1"/>
+      <c r="BRV3" s="1"/>
+      <c r="BSD3" s="1"/>
+      <c r="BSL3" s="1"/>
+      <c r="BST3" s="1"/>
+      <c r="BTB3" s="1"/>
+      <c r="BTJ3" s="1"/>
+      <c r="BTR3" s="1"/>
+      <c r="BTZ3" s="1"/>
+      <c r="BUH3" s="1"/>
+      <c r="BUP3" s="1"/>
+      <c r="BUX3" s="1"/>
+      <c r="BVF3" s="1"/>
+      <c r="BVN3" s="1"/>
+      <c r="BVV3" s="1"/>
+      <c r="BWD3" s="1"/>
+      <c r="BWL3" s="1"/>
+      <c r="BWT3" s="1"/>
+      <c r="BXB3" s="1"/>
+      <c r="BXJ3" s="1"/>
+      <c r="BXR3" s="1"/>
+      <c r="BXZ3" s="1"/>
+      <c r="BYH3" s="1"/>
+      <c r="BYP3" s="1"/>
+      <c r="BYX3" s="1"/>
+      <c r="BZF3" s="1"/>
+      <c r="BZN3" s="1"/>
+      <c r="BZV3" s="1"/>
+      <c r="CAD3" s="1"/>
+      <c r="CAL3" s="1"/>
+      <c r="CAT3" s="1"/>
+      <c r="CBB3" s="1"/>
+      <c r="CBJ3" s="1"/>
+      <c r="CBR3" s="1"/>
+      <c r="CBZ3" s="1"/>
+      <c r="CCH3" s="1"/>
+      <c r="CCP3" s="1"/>
+      <c r="CCX3" s="1"/>
+      <c r="CDF3" s="1"/>
+      <c r="CDN3" s="1"/>
+      <c r="CDV3" s="1"/>
+      <c r="CED3" s="1"/>
+      <c r="CEL3" s="1"/>
+      <c r="CET3" s="1"/>
+      <c r="CFB3" s="1"/>
+      <c r="CFJ3" s="1"/>
+      <c r="CFR3" s="1"/>
+      <c r="CFZ3" s="1"/>
+      <c r="CGH3" s="1"/>
+      <c r="CGP3" s="1"/>
+      <c r="CGX3" s="1"/>
+      <c r="CHF3" s="1"/>
+      <c r="CHN3" s="1"/>
+      <c r="CHV3" s="1"/>
+      <c r="CID3" s="1"/>
+      <c r="CIL3" s="1"/>
+      <c r="CIT3" s="1"/>
+      <c r="CJB3" s="1"/>
+      <c r="CJJ3" s="1"/>
+      <c r="CJR3" s="1"/>
+      <c r="CJZ3" s="1"/>
+      <c r="CKH3" s="1"/>
+      <c r="CKP3" s="1"/>
+      <c r="CKX3" s="1"/>
+      <c r="CLF3" s="1"/>
+      <c r="CLN3" s="1"/>
+      <c r="CLV3" s="1"/>
+      <c r="CMD3" s="1"/>
+      <c r="CML3" s="1"/>
+      <c r="CMT3" s="1"/>
+      <c r="CNB3" s="1"/>
+      <c r="CNJ3" s="1"/>
+      <c r="CNR3" s="1"/>
+      <c r="CNZ3" s="1"/>
+      <c r="COH3" s="1"/>
+      <c r="COP3" s="1"/>
+      <c r="COX3" s="1"/>
+      <c r="CPF3" s="1"/>
+      <c r="CPN3" s="1"/>
+      <c r="CPV3" s="1"/>
+      <c r="CQD3" s="1"/>
+      <c r="CQL3" s="1"/>
+      <c r="CQT3" s="1"/>
+      <c r="CRB3" s="1"/>
+      <c r="CRJ3" s="1"/>
+      <c r="CRR3" s="1"/>
+      <c r="CRZ3" s="1"/>
+      <c r="CSH3" s="1"/>
+      <c r="CSP3" s="1"/>
+      <c r="CSX3" s="1"/>
+      <c r="CTF3" s="1"/>
+      <c r="CTN3" s="1"/>
+      <c r="CTV3" s="1"/>
+      <c r="CUD3" s="1"/>
+      <c r="CUL3" s="1"/>
+      <c r="CUT3" s="1"/>
+      <c r="CVB3" s="1"/>
+      <c r="CVJ3" s="1"/>
+      <c r="CVR3" s="1"/>
+      <c r="CVZ3" s="1"/>
+      <c r="CWH3" s="1"/>
+      <c r="CWP3" s="1"/>
+      <c r="CWX3" s="1"/>
+      <c r="CXF3" s="1"/>
+      <c r="CXN3" s="1"/>
+      <c r="CXV3" s="1"/>
+      <c r="CYD3" s="1"/>
+      <c r="CYL3" s="1"/>
+      <c r="CYT3" s="1"/>
+      <c r="CZB3" s="1"/>
+      <c r="CZJ3" s="1"/>
+      <c r="CZR3" s="1"/>
+      <c r="CZZ3" s="1"/>
+      <c r="DAH3" s="1"/>
+      <c r="DAP3" s="1"/>
+      <c r="DAX3" s="1"/>
+      <c r="DBF3" s="1"/>
+      <c r="DBN3" s="1"/>
+      <c r="DBV3" s="1"/>
+      <c r="DCD3" s="1"/>
+      <c r="DCL3" s="1"/>
+      <c r="DCT3" s="1"/>
+      <c r="DDB3" s="1"/>
+      <c r="DDJ3" s="1"/>
+      <c r="DDR3" s="1"/>
+      <c r="DDZ3" s="1"/>
+      <c r="DEH3" s="1"/>
+      <c r="DEP3" s="1"/>
+      <c r="DEX3" s="1"/>
+      <c r="DFF3" s="1"/>
+      <c r="DFN3" s="1"/>
+      <c r="DFV3" s="1"/>
+      <c r="DGD3" s="1"/>
+      <c r="DGL3" s="1"/>
+      <c r="DGT3" s="1"/>
+      <c r="DHB3" s="1"/>
+      <c r="DHJ3" s="1"/>
+      <c r="DHR3" s="1"/>
+      <c r="DHZ3" s="1"/>
+      <c r="DIH3" s="1"/>
+      <c r="DIP3" s="1"/>
+      <c r="DIX3" s="1"/>
+      <c r="DJF3" s="1"/>
+      <c r="DJN3" s="1"/>
+      <c r="DJV3" s="1"/>
+      <c r="DKD3" s="1"/>
+      <c r="DKL3" s="1"/>
+      <c r="DKT3" s="1"/>
+      <c r="DLB3" s="1"/>
+      <c r="DLJ3" s="1"/>
+      <c r="DLR3" s="1"/>
+      <c r="DLZ3" s="1"/>
+      <c r="DMH3" s="1"/>
+      <c r="DMP3" s="1"/>
+      <c r="DMX3" s="1"/>
+      <c r="DNF3" s="1"/>
+      <c r="DNN3" s="1"/>
+      <c r="DNV3" s="1"/>
+      <c r="DOD3" s="1"/>
+      <c r="DOL3" s="1"/>
+      <c r="DOT3" s="1"/>
+      <c r="DPB3" s="1"/>
+      <c r="DPJ3" s="1"/>
+      <c r="DPR3" s="1"/>
+      <c r="DPZ3" s="1"/>
+      <c r="DQH3" s="1"/>
+      <c r="DQP3" s="1"/>
+      <c r="DQX3" s="1"/>
+      <c r="DRF3" s="1"/>
+      <c r="DRN3" s="1"/>
+      <c r="DRV3" s="1"/>
+      <c r="DSD3" s="1"/>
+      <c r="DSL3" s="1"/>
+      <c r="DST3" s="1"/>
+      <c r="DTB3" s="1"/>
+      <c r="DTJ3" s="1"/>
+      <c r="DTR3" s="1"/>
+      <c r="DTZ3" s="1"/>
+      <c r="DUH3" s="1"/>
+      <c r="DUP3" s="1"/>
+      <c r="DUX3" s="1"/>
+      <c r="DVF3" s="1"/>
+      <c r="DVN3" s="1"/>
+      <c r="DVV3" s="1"/>
+      <c r="DWD3" s="1"/>
+      <c r="DWL3" s="1"/>
+      <c r="DWT3" s="1"/>
+      <c r="DXB3" s="1"/>
+      <c r="DXJ3" s="1"/>
+      <c r="DXR3" s="1"/>
+      <c r="DXZ3" s="1"/>
+      <c r="DYH3" s="1"/>
+      <c r="DYP3" s="1"/>
+      <c r="DYX3" s="1"/>
+      <c r="DZF3" s="1"/>
+      <c r="DZN3" s="1"/>
+      <c r="DZV3" s="1"/>
+      <c r="EAD3" s="1"/>
+      <c r="EAL3" s="1"/>
+      <c r="EAT3" s="1"/>
+      <c r="EBB3" s="1"/>
+      <c r="EBJ3" s="1"/>
+      <c r="EBR3" s="1"/>
+      <c r="EBZ3" s="1"/>
+      <c r="ECH3" s="1"/>
+      <c r="ECP3" s="1"/>
+      <c r="ECX3" s="1"/>
+      <c r="EDF3" s="1"/>
+      <c r="EDN3" s="1"/>
+      <c r="EDV3" s="1"/>
+      <c r="EED3" s="1"/>
+      <c r="EEL3" s="1"/>
+      <c r="EET3" s="1"/>
+      <c r="EFB3" s="1"/>
+      <c r="EFJ3" s="1"/>
+      <c r="EFR3" s="1"/>
+      <c r="EFZ3" s="1"/>
+      <c r="EGH3" s="1"/>
+      <c r="EGP3" s="1"/>
+      <c r="EGX3" s="1"/>
+      <c r="EHF3" s="1"/>
+      <c r="EHN3" s="1"/>
+      <c r="EHV3" s="1"/>
+      <c r="EID3" s="1"/>
+      <c r="EIL3" s="1"/>
+      <c r="EIT3" s="1"/>
+      <c r="EJB3" s="1"/>
+      <c r="EJJ3" s="1"/>
+      <c r="EJR3" s="1"/>
+      <c r="EJZ3" s="1"/>
+      <c r="EKH3" s="1"/>
+      <c r="EKP3" s="1"/>
+      <c r="EKX3" s="1"/>
+      <c r="ELF3" s="1"/>
+      <c r="ELN3" s="1"/>
+      <c r="ELV3" s="1"/>
+      <c r="EMD3" s="1"/>
+      <c r="EML3" s="1"/>
+      <c r="EMT3" s="1"/>
+      <c r="ENB3" s="1"/>
+      <c r="ENJ3" s="1"/>
+      <c r="ENR3" s="1"/>
+      <c r="ENZ3" s="1"/>
+      <c r="EOH3" s="1"/>
+      <c r="EOP3" s="1"/>
+      <c r="EOX3" s="1"/>
+      <c r="EPF3" s="1"/>
+      <c r="EPN3" s="1"/>
+      <c r="EPV3" s="1"/>
+      <c r="EQD3" s="1"/>
+      <c r="EQL3" s="1"/>
+      <c r="EQT3" s="1"/>
+      <c r="ERB3" s="1"/>
+      <c r="ERJ3" s="1"/>
+      <c r="ERR3" s="1"/>
+      <c r="ERZ3" s="1"/>
+      <c r="ESH3" s="1"/>
+      <c r="ESP3" s="1"/>
+      <c r="ESX3" s="1"/>
+      <c r="ETF3" s="1"/>
+      <c r="ETN3" s="1"/>
+      <c r="ETV3" s="1"/>
+      <c r="EUD3" s="1"/>
+      <c r="EUL3" s="1"/>
+      <c r="EUT3" s="1"/>
+      <c r="EVB3" s="1"/>
+      <c r="EVJ3" s="1"/>
+      <c r="EVR3" s="1"/>
+      <c r="EVZ3" s="1"/>
+      <c r="EWH3" s="1"/>
+      <c r="EWP3" s="1"/>
+      <c r="EWX3" s="1"/>
+      <c r="EXF3" s="1"/>
+      <c r="EXN3" s="1"/>
+      <c r="EXV3" s="1"/>
+      <c r="EYD3" s="1"/>
+      <c r="EYL3" s="1"/>
+      <c r="EYT3" s="1"/>
+      <c r="EZB3" s="1"/>
+      <c r="EZJ3" s="1"/>
+      <c r="EZR3" s="1"/>
+      <c r="EZZ3" s="1"/>
+      <c r="FAH3" s="1"/>
+      <c r="FAP3" s="1"/>
+      <c r="FAX3" s="1"/>
+      <c r="FBF3" s="1"/>
+      <c r="FBN3" s="1"/>
+      <c r="FBV3" s="1"/>
+      <c r="FCD3" s="1"/>
+      <c r="FCL3" s="1"/>
+      <c r="FCT3" s="1"/>
+      <c r="FDB3" s="1"/>
+      <c r="FDJ3" s="1"/>
+      <c r="FDR3" s="1"/>
+      <c r="FDZ3" s="1"/>
+      <c r="FEH3" s="1"/>
+      <c r="FEP3" s="1"/>
+      <c r="FEX3" s="1"/>
+      <c r="FFF3" s="1"/>
+      <c r="FFN3" s="1"/>
+      <c r="FFV3" s="1"/>
+      <c r="FGD3" s="1"/>
+      <c r="FGL3" s="1"/>
+      <c r="FGT3" s="1"/>
+      <c r="FHB3" s="1"/>
+      <c r="FHJ3" s="1"/>
+      <c r="FHR3" s="1"/>
+      <c r="FHZ3" s="1"/>
+      <c r="FIH3" s="1"/>
+      <c r="FIP3" s="1"/>
+      <c r="FIX3" s="1"/>
+      <c r="FJF3" s="1"/>
+      <c r="FJN3" s="1"/>
+      <c r="FJV3" s="1"/>
+      <c r="FKD3" s="1"/>
+      <c r="FKL3" s="1"/>
+      <c r="FKT3" s="1"/>
+      <c r="FLB3" s="1"/>
+      <c r="FLJ3" s="1"/>
+      <c r="FLR3" s="1"/>
+      <c r="FLZ3" s="1"/>
+      <c r="FMH3" s="1"/>
+      <c r="FMP3" s="1"/>
+      <c r="FMX3" s="1"/>
+      <c r="FNF3" s="1"/>
+      <c r="FNN3" s="1"/>
+      <c r="FNV3" s="1"/>
+      <c r="FOD3" s="1"/>
+      <c r="FOL3" s="1"/>
+      <c r="FOT3" s="1"/>
+      <c r="FPB3" s="1"/>
+      <c r="FPJ3" s="1"/>
+      <c r="FPR3" s="1"/>
+      <c r="FPZ3" s="1"/>
+      <c r="FQH3" s="1"/>
+      <c r="FQP3" s="1"/>
+      <c r="FQX3" s="1"/>
+      <c r="FRF3" s="1"/>
+      <c r="FRN3" s="1"/>
+      <c r="FRV3" s="1"/>
+      <c r="FSD3" s="1"/>
+      <c r="FSL3" s="1"/>
+      <c r="FST3" s="1"/>
+      <c r="FTB3" s="1"/>
+      <c r="FTJ3" s="1"/>
+      <c r="FTR3" s="1"/>
+      <c r="FTZ3" s="1"/>
+      <c r="FUH3" s="1"/>
+      <c r="FUP3" s="1"/>
+      <c r="FUX3" s="1"/>
+      <c r="FVF3" s="1"/>
+      <c r="FVN3" s="1"/>
+      <c r="FVV3" s="1"/>
+      <c r="FWD3" s="1"/>
+      <c r="FWL3" s="1"/>
+      <c r="FWT3" s="1"/>
+      <c r="FXB3" s="1"/>
+      <c r="FXJ3" s="1"/>
+      <c r="FXR3" s="1"/>
+      <c r="FXZ3" s="1"/>
+      <c r="FYH3" s="1"/>
+      <c r="FYP3" s="1"/>
+      <c r="FYX3" s="1"/>
+      <c r="FZF3" s="1"/>
+      <c r="FZN3" s="1"/>
+      <c r="FZV3" s="1"/>
+      <c r="GAD3" s="1"/>
+      <c r="GAL3" s="1"/>
+      <c r="GAT3" s="1"/>
+      <c r="GBB3" s="1"/>
+      <c r="GBJ3" s="1"/>
+      <c r="GBR3" s="1"/>
+      <c r="GBZ3" s="1"/>
+      <c r="GCH3" s="1"/>
+      <c r="GCP3" s="1"/>
+      <c r="GCX3" s="1"/>
+      <c r="GDF3" s="1"/>
+      <c r="GDN3" s="1"/>
+      <c r="GDV3" s="1"/>
+      <c r="GED3" s="1"/>
+      <c r="GEL3" s="1"/>
+      <c r="GET3" s="1"/>
+      <c r="GFB3" s="1"/>
+      <c r="GFJ3" s="1"/>
+      <c r="GFR3" s="1"/>
+      <c r="GFZ3" s="1"/>
+      <c r="GGH3" s="1"/>
+      <c r="GGP3" s="1"/>
+      <c r="GGX3" s="1"/>
+      <c r="GHF3" s="1"/>
+      <c r="GHN3" s="1"/>
+      <c r="GHV3" s="1"/>
+      <c r="GID3" s="1"/>
+      <c r="GIL3" s="1"/>
+      <c r="GIT3" s="1"/>
+      <c r="GJB3" s="1"/>
+      <c r="GJJ3" s="1"/>
+      <c r="GJR3" s="1"/>
+      <c r="GJZ3" s="1"/>
+      <c r="GKH3" s="1"/>
+      <c r="GKP3" s="1"/>
+      <c r="GKX3" s="1"/>
+      <c r="GLF3" s="1"/>
+      <c r="GLN3" s="1"/>
+      <c r="GLV3" s="1"/>
+      <c r="GMD3" s="1"/>
+      <c r="GML3" s="1"/>
+      <c r="GMT3" s="1"/>
+      <c r="GNB3" s="1"/>
+      <c r="GNJ3" s="1"/>
+      <c r="GNR3" s="1"/>
+      <c r="GNZ3" s="1"/>
+      <c r="GOH3" s="1"/>
+      <c r="GOP3" s="1"/>
+      <c r="GOX3" s="1"/>
+      <c r="GPF3" s="1"/>
+      <c r="GPN3" s="1"/>
+      <c r="GPV3" s="1"/>
+      <c r="GQD3" s="1"/>
+      <c r="GQL3" s="1"/>
+      <c r="GQT3" s="1"/>
+      <c r="GRB3" s="1"/>
+      <c r="GRJ3" s="1"/>
+      <c r="GRR3" s="1"/>
+      <c r="GRZ3" s="1"/>
+      <c r="GSH3" s="1"/>
+      <c r="GSP3" s="1"/>
+      <c r="GSX3" s="1"/>
+      <c r="GTF3" s="1"/>
+      <c r="GTN3" s="1"/>
+      <c r="GTV3" s="1"/>
+      <c r="GUD3" s="1"/>
+      <c r="GUL3" s="1"/>
+      <c r="GUT3" s="1"/>
+      <c r="GVB3" s="1"/>
+      <c r="GVJ3" s="1"/>
+      <c r="GVR3" s="1"/>
+      <c r="GVZ3" s="1"/>
+      <c r="GWH3" s="1"/>
+      <c r="GWP3" s="1"/>
+      <c r="GWX3" s="1"/>
+      <c r="GXF3" s="1"/>
+      <c r="GXN3" s="1"/>
+      <c r="GXV3" s="1"/>
+      <c r="GYD3" s="1"/>
+      <c r="GYL3" s="1"/>
+      <c r="GYT3" s="1"/>
+      <c r="GZB3" s="1"/>
+      <c r="GZJ3" s="1"/>
+      <c r="GZR3" s="1"/>
+      <c r="GZZ3" s="1"/>
+      <c r="HAH3" s="1"/>
+      <c r="HAP3" s="1"/>
+      <c r="HAX3" s="1"/>
+      <c r="HBF3" s="1"/>
+      <c r="HBN3" s="1"/>
+      <c r="HBV3" s="1"/>
+      <c r="HCD3" s="1"/>
+      <c r="HCL3" s="1"/>
+      <c r="HCT3" s="1"/>
+      <c r="HDB3" s="1"/>
+      <c r="HDJ3" s="1"/>
+      <c r="HDR3" s="1"/>
+      <c r="HDZ3" s="1"/>
+      <c r="HEH3" s="1"/>
+      <c r="HEP3" s="1"/>
+      <c r="HEX3" s="1"/>
+      <c r="HFF3" s="1"/>
+      <c r="HFN3" s="1"/>
+      <c r="HFV3" s="1"/>
+      <c r="HGD3" s="1"/>
+      <c r="HGL3" s="1"/>
+      <c r="HGT3" s="1"/>
+      <c r="HHB3" s="1"/>
+      <c r="HHJ3" s="1"/>
+      <c r="HHR3" s="1"/>
+      <c r="HHZ3" s="1"/>
+      <c r="HIH3" s="1"/>
+      <c r="HIP3" s="1"/>
+      <c r="HIX3" s="1"/>
+      <c r="HJF3" s="1"/>
+      <c r="HJN3" s="1"/>
+      <c r="HJV3" s="1"/>
+      <c r="HKD3" s="1"/>
+      <c r="HKL3" s="1"/>
+      <c r="HKT3" s="1"/>
+      <c r="HLB3" s="1"/>
+      <c r="HLJ3" s="1"/>
+      <c r="HLR3" s="1"/>
+      <c r="HLZ3" s="1"/>
+      <c r="HMH3" s="1"/>
+      <c r="HMP3" s="1"/>
+      <c r="HMX3" s="1"/>
+      <c r="HNF3" s="1"/>
+      <c r="HNN3" s="1"/>
+      <c r="HNV3" s="1"/>
+      <c r="HOD3" s="1"/>
+      <c r="HOL3" s="1"/>
+      <c r="HOT3" s="1"/>
+      <c r="HPB3" s="1"/>
+      <c r="HPJ3" s="1"/>
+      <c r="HPR3" s="1"/>
+      <c r="HPZ3" s="1"/>
+      <c r="HQH3" s="1"/>
+      <c r="HQP3" s="1"/>
+      <c r="HQX3" s="1"/>
+      <c r="HRF3" s="1"/>
+      <c r="HRN3" s="1"/>
+      <c r="HRV3" s="1"/>
+      <c r="HSD3" s="1"/>
+      <c r="HSL3" s="1"/>
+      <c r="HST3" s="1"/>
+      <c r="HTB3" s="1"/>
+      <c r="HTJ3" s="1"/>
+      <c r="HTR3" s="1"/>
+      <c r="HTZ3" s="1"/>
+      <c r="HUH3" s="1"/>
+      <c r="HUP3" s="1"/>
+      <c r="HUX3" s="1"/>
+      <c r="HVF3" s="1"/>
+      <c r="HVN3" s="1"/>
+      <c r="HVV3" s="1"/>
+      <c r="HWD3" s="1"/>
+      <c r="HWL3" s="1"/>
+      <c r="HWT3" s="1"/>
+      <c r="HXB3" s="1"/>
+      <c r="HXJ3" s="1"/>
+      <c r="HXR3" s="1"/>
+      <c r="HXZ3" s="1"/>
+      <c r="HYH3" s="1"/>
+      <c r="HYP3" s="1"/>
+      <c r="HYX3" s="1"/>
+      <c r="HZF3" s="1"/>
+      <c r="HZN3" s="1"/>
+      <c r="HZV3" s="1"/>
+      <c r="IAD3" s="1"/>
+      <c r="IAL3" s="1"/>
+      <c r="IAT3" s="1"/>
+      <c r="IBB3" s="1"/>
+      <c r="IBJ3" s="1"/>
+      <c r="IBR3" s="1"/>
+      <c r="IBZ3" s="1"/>
+      <c r="ICH3" s="1"/>
+      <c r="ICP3" s="1"/>
+      <c r="ICX3" s="1"/>
+      <c r="IDF3" s="1"/>
+      <c r="IDN3" s="1"/>
+      <c r="IDV3" s="1"/>
+      <c r="IED3" s="1"/>
+      <c r="IEL3" s="1"/>
+      <c r="IET3" s="1"/>
+      <c r="IFB3" s="1"/>
+      <c r="IFJ3" s="1"/>
+      <c r="IFR3" s="1"/>
+      <c r="IFZ3" s="1"/>
+      <c r="IGH3" s="1"/>
+      <c r="IGP3" s="1"/>
+      <c r="IGX3" s="1"/>
+      <c r="IHF3" s="1"/>
+      <c r="IHN3" s="1"/>
+      <c r="IHV3" s="1"/>
+      <c r="IID3" s="1"/>
+      <c r="IIL3" s="1"/>
+      <c r="IIT3" s="1"/>
+      <c r="IJB3" s="1"/>
+      <c r="IJJ3" s="1"/>
+      <c r="IJR3" s="1"/>
+      <c r="IJZ3" s="1"/>
+      <c r="IKH3" s="1"/>
+      <c r="IKP3" s="1"/>
+      <c r="IKX3" s="1"/>
+      <c r="ILF3" s="1"/>
+      <c r="ILN3" s="1"/>
+      <c r="ILV3" s="1"/>
+      <c r="IMD3" s="1"/>
+      <c r="IML3" s="1"/>
+      <c r="IMT3" s="1"/>
+      <c r="INB3" s="1"/>
+      <c r="INJ3" s="1"/>
+      <c r="INR3" s="1"/>
+      <c r="INZ3" s="1"/>
+      <c r="IOH3" s="1"/>
+      <c r="IOP3" s="1"/>
+      <c r="IOX3" s="1"/>
+      <c r="IPF3" s="1"/>
+      <c r="IPN3" s="1"/>
+      <c r="IPV3" s="1"/>
+      <c r="IQD3" s="1"/>
+      <c r="IQL3" s="1"/>
+      <c r="IQT3" s="1"/>
+      <c r="IRB3" s="1"/>
+      <c r="IRJ3" s="1"/>
+      <c r="IRR3" s="1"/>
+      <c r="IRZ3" s="1"/>
+      <c r="ISH3" s="1"/>
+      <c r="ISP3" s="1"/>
+      <c r="ISX3" s="1"/>
+      <c r="ITF3" s="1"/>
+      <c r="ITN3" s="1"/>
+      <c r="ITV3" s="1"/>
+      <c r="IUD3" s="1"/>
+      <c r="IUL3" s="1"/>
+      <c r="IUT3" s="1"/>
+      <c r="IVB3" s="1"/>
+      <c r="IVJ3" s="1"/>
+      <c r="IVR3" s="1"/>
+      <c r="IVZ3" s="1"/>
+      <c r="IWH3" s="1"/>
+      <c r="IWP3" s="1"/>
+      <c r="IWX3" s="1"/>
+      <c r="IXF3" s="1"/>
+      <c r="IXN3" s="1"/>
+      <c r="IXV3" s="1"/>
+      <c r="IYD3" s="1"/>
+      <c r="IYL3" s="1"/>
+      <c r="IYT3" s="1"/>
+      <c r="IZB3" s="1"/>
+      <c r="IZJ3" s="1"/>
+      <c r="IZR3" s="1"/>
+      <c r="IZZ3" s="1"/>
+      <c r="JAH3" s="1"/>
+      <c r="JAP3" s="1"/>
+      <c r="JAX3" s="1"/>
+      <c r="JBF3" s="1"/>
+      <c r="JBN3" s="1"/>
+      <c r="JBV3" s="1"/>
+      <c r="JCD3" s="1"/>
+      <c r="JCL3" s="1"/>
+      <c r="JCT3" s="1"/>
+      <c r="JDB3" s="1"/>
+      <c r="JDJ3" s="1"/>
+      <c r="JDR3" s="1"/>
+      <c r="JDZ3" s="1"/>
+      <c r="JEH3" s="1"/>
+      <c r="JEP3" s="1"/>
+      <c r="JEX3" s="1"/>
+      <c r="JFF3" s="1"/>
+      <c r="JFN3" s="1"/>
+      <c r="JFV3" s="1"/>
+      <c r="JGD3" s="1"/>
+      <c r="JGL3" s="1"/>
+      <c r="JGT3" s="1"/>
+      <c r="JHB3" s="1"/>
+      <c r="JHJ3" s="1"/>
+      <c r="JHR3" s="1"/>
+      <c r="JHZ3" s="1"/>
+      <c r="JIH3" s="1"/>
+      <c r="JIP3" s="1"/>
+      <c r="JIX3" s="1"/>
+      <c r="JJF3" s="1"/>
+      <c r="JJN3" s="1"/>
+      <c r="JJV3" s="1"/>
+      <c r="JKD3" s="1"/>
+      <c r="JKL3" s="1"/>
+      <c r="JKT3" s="1"/>
+      <c r="JLB3" s="1"/>
+      <c r="JLJ3" s="1"/>
+      <c r="JLR3" s="1"/>
+      <c r="JLZ3" s="1"/>
+      <c r="JMH3" s="1"/>
+      <c r="JMP3" s="1"/>
+      <c r="JMX3" s="1"/>
+      <c r="JNF3" s="1"/>
+      <c r="JNN3" s="1"/>
+      <c r="JNV3" s="1"/>
+      <c r="JOD3" s="1"/>
+      <c r="JOL3" s="1"/>
+      <c r="JOT3" s="1"/>
+      <c r="JPB3" s="1"/>
+      <c r="JPJ3" s="1"/>
+      <c r="JPR3" s="1"/>
+      <c r="JPZ3" s="1"/>
+      <c r="JQH3" s="1"/>
+      <c r="JQP3" s="1"/>
+      <c r="JQX3" s="1"/>
+      <c r="JRF3" s="1"/>
+      <c r="JRN3" s="1"/>
+      <c r="JRV3" s="1"/>
+      <c r="JSD3" s="1"/>
+      <c r="JSL3" s="1"/>
+      <c r="JST3" s="1"/>
+      <c r="JTB3" s="1"/>
+      <c r="JTJ3" s="1"/>
+      <c r="JTR3" s="1"/>
+      <c r="JTZ3" s="1"/>
+      <c r="JUH3" s="1"/>
+      <c r="JUP3" s="1"/>
+      <c r="JUX3" s="1"/>
+      <c r="JVF3" s="1"/>
+      <c r="JVN3" s="1"/>
+      <c r="JVV3" s="1"/>
+      <c r="JWD3" s="1"/>
+      <c r="JWL3" s="1"/>
+      <c r="JWT3" s="1"/>
+      <c r="JXB3" s="1"/>
+      <c r="JXJ3" s="1"/>
+      <c r="JXR3" s="1"/>
+      <c r="JXZ3" s="1"/>
+      <c r="JYH3" s="1"/>
+      <c r="JYP3" s="1"/>
+      <c r="JYX3" s="1"/>
+      <c r="JZF3" s="1"/>
+      <c r="JZN3" s="1"/>
+      <c r="JZV3" s="1"/>
+      <c r="KAD3" s="1"/>
+      <c r="KAL3" s="1"/>
+      <c r="KAT3" s="1"/>
+      <c r="KBB3" s="1"/>
+      <c r="KBJ3" s="1"/>
+      <c r="KBR3" s="1"/>
+      <c r="KBZ3" s="1"/>
+      <c r="KCH3" s="1"/>
+      <c r="KCP3" s="1"/>
+      <c r="KCX3" s="1"/>
+      <c r="KDF3" s="1"/>
+      <c r="KDN3" s="1"/>
+      <c r="KDV3" s="1"/>
+      <c r="KED3" s="1"/>
+      <c r="KEL3" s="1"/>
+      <c r="KET3" s="1"/>
+      <c r="KFB3" s="1"/>
+      <c r="KFJ3" s="1"/>
+      <c r="KFR3" s="1"/>
+      <c r="KFZ3" s="1"/>
+      <c r="KGH3" s="1"/>
+      <c r="KGP3" s="1"/>
+      <c r="KGX3" s="1"/>
+      <c r="KHF3" s="1"/>
+      <c r="KHN3" s="1"/>
+      <c r="KHV3" s="1"/>
+      <c r="KID3" s="1"/>
+      <c r="KIL3" s="1"/>
+      <c r="KIT3" s="1"/>
+      <c r="KJB3" s="1"/>
+      <c r="KJJ3" s="1"/>
+      <c r="KJR3" s="1"/>
+      <c r="KJZ3" s="1"/>
+      <c r="KKH3" s="1"/>
+      <c r="KKP3" s="1"/>
+      <c r="KKX3" s="1"/>
+      <c r="KLF3" s="1"/>
+      <c r="KLN3" s="1"/>
+      <c r="KLV3" s="1"/>
+      <c r="KMD3" s="1"/>
+      <c r="KML3" s="1"/>
+      <c r="KMT3" s="1"/>
+      <c r="KNB3" s="1"/>
+      <c r="KNJ3" s="1"/>
+      <c r="KNR3" s="1"/>
+      <c r="KNZ3" s="1"/>
+      <c r="KOH3" s="1"/>
+      <c r="KOP3" s="1"/>
+      <c r="KOX3" s="1"/>
+      <c r="KPF3" s="1"/>
+      <c r="KPN3" s="1"/>
+      <c r="KPV3" s="1"/>
+      <c r="KQD3" s="1"/>
+      <c r="KQL3" s="1"/>
+      <c r="KQT3" s="1"/>
+      <c r="KRB3" s="1"/>
+      <c r="KRJ3" s="1"/>
+      <c r="KRR3" s="1"/>
+      <c r="KRZ3" s="1"/>
+      <c r="KSH3" s="1"/>
+      <c r="KSP3" s="1"/>
+      <c r="KSX3" s="1"/>
+      <c r="KTF3" s="1"/>
+      <c r="KTN3" s="1"/>
+      <c r="KTV3" s="1"/>
+      <c r="KUD3" s="1"/>
+      <c r="KUL3" s="1"/>
+      <c r="KUT3" s="1"/>
+      <c r="KVB3" s="1"/>
+      <c r="KVJ3" s="1"/>
+      <c r="KVR3" s="1"/>
+      <c r="KVZ3" s="1"/>
+      <c r="KWH3" s="1"/>
+      <c r="KWP3" s="1"/>
+      <c r="KWX3" s="1"/>
+      <c r="KXF3" s="1"/>
+      <c r="KXN3" s="1"/>
+      <c r="KXV3" s="1"/>
+      <c r="KYD3" s="1"/>
+      <c r="KYL3" s="1"/>
+      <c r="KYT3" s="1"/>
+      <c r="KZB3" s="1"/>
+      <c r="KZJ3" s="1"/>
+      <c r="KZR3" s="1"/>
+      <c r="KZZ3" s="1"/>
+      <c r="LAH3" s="1"/>
+      <c r="LAP3" s="1"/>
+      <c r="LAX3" s="1"/>
+      <c r="LBF3" s="1"/>
+      <c r="LBN3" s="1"/>
+      <c r="LBV3" s="1"/>
+      <c r="LCD3" s="1"/>
+      <c r="LCL3" s="1"/>
+      <c r="LCT3" s="1"/>
+      <c r="LDB3" s="1"/>
+      <c r="LDJ3" s="1"/>
+      <c r="LDR3" s="1"/>
+      <c r="LDZ3" s="1"/>
+      <c r="LEH3" s="1"/>
+      <c r="LEP3" s="1"/>
+      <c r="LEX3" s="1"/>
+      <c r="LFF3" s="1"/>
+      <c r="LFN3" s="1"/>
+      <c r="LFV3" s="1"/>
+      <c r="LGD3" s="1"/>
+      <c r="LGL3" s="1"/>
+      <c r="LGT3" s="1"/>
+      <c r="LHB3" s="1"/>
+      <c r="LHJ3" s="1"/>
+      <c r="LHR3" s="1"/>
+      <c r="LHZ3" s="1"/>
+      <c r="LIH3" s="1"/>
+      <c r="LIP3" s="1"/>
+      <c r="LIX3" s="1"/>
+      <c r="LJF3" s="1"/>
+      <c r="LJN3" s="1"/>
+      <c r="LJV3" s="1"/>
+      <c r="LKD3" s="1"/>
+      <c r="LKL3" s="1"/>
+      <c r="LKT3" s="1"/>
+      <c r="LLB3" s="1"/>
+      <c r="LLJ3" s="1"/>
+      <c r="LLR3" s="1"/>
+      <c r="LLZ3" s="1"/>
+      <c r="LMH3" s="1"/>
+      <c r="LMP3" s="1"/>
+      <c r="LMX3" s="1"/>
+      <c r="LNF3" s="1"/>
+      <c r="LNN3" s="1"/>
+      <c r="LNV3" s="1"/>
+      <c r="LOD3" s="1"/>
+      <c r="LOL3" s="1"/>
+      <c r="LOT3" s="1"/>
+      <c r="LPB3" s="1"/>
+      <c r="LPJ3" s="1"/>
+      <c r="LPR3" s="1"/>
+      <c r="LPZ3" s="1"/>
+      <c r="LQH3" s="1"/>
+      <c r="LQP3" s="1"/>
+      <c r="LQX3" s="1"/>
+      <c r="LRF3" s="1"/>
+      <c r="LRN3" s="1"/>
+      <c r="LRV3" s="1"/>
+      <c r="LSD3" s="1"/>
+      <c r="LSL3" s="1"/>
+      <c r="LST3" s="1"/>
+      <c r="LTB3" s="1"/>
+      <c r="LTJ3" s="1"/>
+      <c r="LTR3" s="1"/>
+      <c r="LTZ3" s="1"/>
+      <c r="LUH3" s="1"/>
+      <c r="LUP3" s="1"/>
+      <c r="LUX3" s="1"/>
+      <c r="LVF3" s="1"/>
+      <c r="LVN3" s="1"/>
+      <c r="LVV3" s="1"/>
+      <c r="LWD3" s="1"/>
+      <c r="LWL3" s="1"/>
+      <c r="LWT3" s="1"/>
+      <c r="LXB3" s="1"/>
+      <c r="LXJ3" s="1"/>
+      <c r="LXR3" s="1"/>
+      <c r="LXZ3" s="1"/>
+      <c r="LYH3" s="1"/>
+      <c r="LYP3" s="1"/>
+      <c r="LYX3" s="1"/>
+      <c r="LZF3" s="1"/>
+      <c r="LZN3" s="1"/>
+      <c r="LZV3" s="1"/>
+      <c r="MAD3" s="1"/>
+      <c r="MAL3" s="1"/>
+      <c r="MAT3" s="1"/>
+      <c r="MBB3" s="1"/>
+      <c r="MBJ3" s="1"/>
+      <c r="MBR3" s="1"/>
+      <c r="MBZ3" s="1"/>
+      <c r="MCH3" s="1"/>
+      <c r="MCP3" s="1"/>
+      <c r="MCX3" s="1"/>
+      <c r="MDF3" s="1"/>
+      <c r="MDN3" s="1"/>
+      <c r="MDV3" s="1"/>
+      <c r="MED3" s="1"/>
+      <c r="MEL3" s="1"/>
+      <c r="MET3" s="1"/>
+      <c r="MFB3" s="1"/>
+      <c r="MFJ3" s="1"/>
+      <c r="MFR3" s="1"/>
+      <c r="MFZ3" s="1"/>
+      <c r="MGH3" s="1"/>
+      <c r="MGP3" s="1"/>
+      <c r="MGX3" s="1"/>
+      <c r="MHF3" s="1"/>
+      <c r="MHN3" s="1"/>
+      <c r="MHV3" s="1"/>
+      <c r="MID3" s="1"/>
+      <c r="MIL3" s="1"/>
+      <c r="MIT3" s="1"/>
+      <c r="MJB3" s="1"/>
+      <c r="MJJ3" s="1"/>
+      <c r="MJR3" s="1"/>
+      <c r="MJZ3" s="1"/>
+      <c r="MKH3" s="1"/>
+      <c r="MKP3" s="1"/>
+      <c r="MKX3" s="1"/>
+      <c r="MLF3" s="1"/>
+      <c r="MLN3" s="1"/>
+      <c r="MLV3" s="1"/>
+      <c r="MMD3" s="1"/>
+      <c r="MML3" s="1"/>
+      <c r="MMT3" s="1"/>
+      <c r="MNB3" s="1"/>
+      <c r="MNJ3" s="1"/>
+      <c r="MNR3" s="1"/>
+      <c r="MNZ3" s="1"/>
+      <c r="MOH3" s="1"/>
+      <c r="MOP3" s="1"/>
+      <c r="MOX3" s="1"/>
+      <c r="MPF3" s="1"/>
+      <c r="MPN3" s="1"/>
+      <c r="MPV3" s="1"/>
+      <c r="MQD3" s="1"/>
+      <c r="MQL3" s="1"/>
+      <c r="MQT3" s="1"/>
+      <c r="MRB3" s="1"/>
+      <c r="MRJ3" s="1"/>
+      <c r="MRR3" s="1"/>
+      <c r="MRZ3" s="1"/>
+      <c r="MSH3" s="1"/>
+      <c r="MSP3" s="1"/>
+      <c r="MSX3" s="1"/>
+      <c r="MTF3" s="1"/>
+      <c r="MTN3" s="1"/>
+      <c r="MTV3" s="1"/>
+      <c r="MUD3" s="1"/>
+      <c r="MUL3" s="1"/>
+      <c r="MUT3" s="1"/>
+      <c r="MVB3" s="1"/>
+      <c r="MVJ3" s="1"/>
+      <c r="MVR3" s="1"/>
+      <c r="MVZ3" s="1"/>
+      <c r="MWH3" s="1"/>
+      <c r="MWP3" s="1"/>
+      <c r="MWX3" s="1"/>
+      <c r="MXF3" s="1"/>
+      <c r="MXN3" s="1"/>
+      <c r="MXV3" s="1"/>
+      <c r="MYD3" s="1"/>
+      <c r="MYL3" s="1"/>
+      <c r="MYT3" s="1"/>
+      <c r="MZB3" s="1"/>
+      <c r="MZJ3" s="1"/>
+      <c r="MZR3" s="1"/>
+      <c r="MZZ3" s="1"/>
+      <c r="NAH3" s="1"/>
+      <c r="NAP3" s="1"/>
+      <c r="NAX3" s="1"/>
+      <c r="NBF3" s="1"/>
+      <c r="NBN3" s="1"/>
+      <c r="NBV3" s="1"/>
+      <c r="NCD3" s="1"/>
+      <c r="NCL3" s="1"/>
+      <c r="NCT3" s="1"/>
+      <c r="NDB3" s="1"/>
+      <c r="NDJ3" s="1"/>
+      <c r="NDR3" s="1"/>
+      <c r="NDZ3" s="1"/>
+      <c r="NEH3" s="1"/>
+      <c r="NEP3" s="1"/>
+      <c r="NEX3" s="1"/>
+      <c r="NFF3" s="1"/>
+      <c r="NFN3" s="1"/>
+      <c r="NFV3" s="1"/>
+      <c r="NGD3" s="1"/>
+      <c r="NGL3" s="1"/>
+      <c r="NGT3" s="1"/>
+      <c r="NHB3" s="1"/>
+      <c r="NHJ3" s="1"/>
+      <c r="NHR3" s="1"/>
+      <c r="NHZ3" s="1"/>
+      <c r="NIH3" s="1"/>
+      <c r="NIP3" s="1"/>
+      <c r="NIX3" s="1"/>
+      <c r="NJF3" s="1"/>
+      <c r="NJN3" s="1"/>
+      <c r="NJV3" s="1"/>
+      <c r="NKD3" s="1"/>
+      <c r="NKL3" s="1"/>
+      <c r="NKT3" s="1"/>
+      <c r="NLB3" s="1"/>
+      <c r="NLJ3" s="1"/>
+      <c r="NLR3" s="1"/>
+      <c r="NLZ3" s="1"/>
+      <c r="NMH3" s="1"/>
+      <c r="NMP3" s="1"/>
+      <c r="NMX3" s="1"/>
+      <c r="NNF3" s="1"/>
+      <c r="NNN3" s="1"/>
+      <c r="NNV3" s="1"/>
+      <c r="NOD3" s="1"/>
+      <c r="NOL3" s="1"/>
+      <c r="NOT3" s="1"/>
+      <c r="NPB3" s="1"/>
+      <c r="NPJ3" s="1"/>
+      <c r="NPR3" s="1"/>
+      <c r="NPZ3" s="1"/>
+      <c r="NQH3" s="1"/>
+      <c r="NQP3" s="1"/>
+      <c r="NQX3" s="1"/>
+      <c r="NRF3" s="1"/>
+      <c r="NRN3" s="1"/>
+      <c r="NRV3" s="1"/>
+      <c r="NSD3" s="1"/>
+      <c r="NSL3" s="1"/>
+      <c r="NST3" s="1"/>
+      <c r="NTB3" s="1"/>
+      <c r="NTJ3" s="1"/>
+      <c r="NTR3" s="1"/>
+      <c r="NTZ3" s="1"/>
+      <c r="NUH3" s="1"/>
+      <c r="NUP3" s="1"/>
+      <c r="NUX3" s="1"/>
+      <c r="NVF3" s="1"/>
+      <c r="NVN3" s="1"/>
+      <c r="NVV3" s="1"/>
+      <c r="NWD3" s="1"/>
+      <c r="NWL3" s="1"/>
+      <c r="NWT3" s="1"/>
+      <c r="NXB3" s="1"/>
+      <c r="NXJ3" s="1"/>
+      <c r="NXR3" s="1"/>
+      <c r="NXZ3" s="1"/>
+      <c r="NYH3" s="1"/>
+      <c r="NYP3" s="1"/>
+      <c r="NYX3" s="1"/>
+      <c r="NZF3" s="1"/>
+      <c r="NZN3" s="1"/>
+      <c r="NZV3" s="1"/>
+      <c r="OAD3" s="1"/>
+      <c r="OAL3" s="1"/>
+      <c r="OAT3" s="1"/>
+      <c r="OBB3" s="1"/>
+      <c r="OBJ3" s="1"/>
+      <c r="OBR3" s="1"/>
+      <c r="OBZ3" s="1"/>
+      <c r="OCH3" s="1"/>
+      <c r="OCP3" s="1"/>
+      <c r="OCX3" s="1"/>
+      <c r="ODF3" s="1"/>
+      <c r="ODN3" s="1"/>
+      <c r="ODV3" s="1"/>
+      <c r="OED3" s="1"/>
+      <c r="OEL3" s="1"/>
+      <c r="OET3" s="1"/>
+      <c r="OFB3" s="1"/>
+      <c r="OFJ3" s="1"/>
+      <c r="OFR3" s="1"/>
+      <c r="OFZ3" s="1"/>
+      <c r="OGH3" s="1"/>
+      <c r="OGP3" s="1"/>
+      <c r="OGX3" s="1"/>
+      <c r="OHF3" s="1"/>
+      <c r="OHN3" s="1"/>
+      <c r="OHV3" s="1"/>
+      <c r="OID3" s="1"/>
+      <c r="OIL3" s="1"/>
+      <c r="OIT3" s="1"/>
+      <c r="OJB3" s="1"/>
+      <c r="OJJ3" s="1"/>
+      <c r="OJR3" s="1"/>
+      <c r="OJZ3" s="1"/>
+      <c r="OKH3" s="1"/>
+      <c r="OKP3" s="1"/>
+      <c r="OKX3" s="1"/>
+      <c r="OLF3" s="1"/>
+      <c r="OLN3" s="1"/>
+      <c r="OLV3" s="1"/>
+      <c r="OMD3" s="1"/>
+      <c r="OML3" s="1"/>
+      <c r="OMT3" s="1"/>
+      <c r="ONB3" s="1"/>
+      <c r="ONJ3" s="1"/>
+      <c r="ONR3" s="1"/>
+      <c r="ONZ3" s="1"/>
+      <c r="OOH3" s="1"/>
+      <c r="OOP3" s="1"/>
+      <c r="OOX3" s="1"/>
+      <c r="OPF3" s="1"/>
+      <c r="OPN3" s="1"/>
+      <c r="OPV3" s="1"/>
+      <c r="OQD3" s="1"/>
+      <c r="OQL3" s="1"/>
+      <c r="OQT3" s="1"/>
+      <c r="ORB3" s="1"/>
+      <c r="ORJ3" s="1"/>
+      <c r="ORR3" s="1"/>
+      <c r="ORZ3" s="1"/>
+      <c r="OSH3" s="1"/>
+      <c r="OSP3" s="1"/>
+      <c r="OSX3" s="1"/>
+      <c r="OTF3" s="1"/>
+      <c r="OTN3" s="1"/>
+      <c r="OTV3" s="1"/>
+      <c r="OUD3" s="1"/>
+      <c r="OUL3" s="1"/>
+      <c r="OUT3" s="1"/>
+      <c r="OVB3" s="1"/>
+      <c r="OVJ3" s="1"/>
+      <c r="OVR3" s="1"/>
+      <c r="OVZ3" s="1"/>
+      <c r="OWH3" s="1"/>
+      <c r="OWP3" s="1"/>
+      <c r="OWX3" s="1"/>
+      <c r="OXF3" s="1"/>
+      <c r="OXN3" s="1"/>
+      <c r="OXV3" s="1"/>
+      <c r="OYD3" s="1"/>
+      <c r="OYL3" s="1"/>
+      <c r="OYT3" s="1"/>
+      <c r="OZB3" s="1"/>
+      <c r="OZJ3" s="1"/>
+      <c r="OZR3" s="1"/>
+      <c r="OZZ3" s="1"/>
+      <c r="PAH3" s="1"/>
+      <c r="PAP3" s="1"/>
+      <c r="PAX3" s="1"/>
+      <c r="PBF3" s="1"/>
+      <c r="PBN3" s="1"/>
+      <c r="PBV3" s="1"/>
+      <c r="PCD3" s="1"/>
+      <c r="PCL3" s="1"/>
+      <c r="PCT3" s="1"/>
+      <c r="PDB3" s="1"/>
+      <c r="PDJ3" s="1"/>
+      <c r="PDR3" s="1"/>
+      <c r="PDZ3" s="1"/>
+      <c r="PEH3" s="1"/>
+      <c r="PEP3" s="1"/>
+      <c r="PEX3" s="1"/>
+      <c r="PFF3" s="1"/>
+      <c r="PFN3" s="1"/>
+      <c r="PFV3" s="1"/>
+      <c r="PGD3" s="1"/>
+      <c r="PGL3" s="1"/>
+      <c r="PGT3" s="1"/>
+      <c r="PHB3" s="1"/>
+      <c r="PHJ3" s="1"/>
+      <c r="PHR3" s="1"/>
+      <c r="PHZ3" s="1"/>
+      <c r="PIH3" s="1"/>
+      <c r="PIP3" s="1"/>
+      <c r="PIX3" s="1"/>
+      <c r="PJF3" s="1"/>
+      <c r="PJN3" s="1"/>
+      <c r="PJV3" s="1"/>
+      <c r="PKD3" s="1"/>
+      <c r="PKL3" s="1"/>
+      <c r="PKT3" s="1"/>
+      <c r="PLB3" s="1"/>
+      <c r="PLJ3" s="1"/>
+      <c r="PLR3" s="1"/>
+      <c r="PLZ3" s="1"/>
+      <c r="PMH3" s="1"/>
+      <c r="PMP3" s="1"/>
+      <c r="PMX3" s="1"/>
+      <c r="PNF3" s="1"/>
+      <c r="PNN3" s="1"/>
+      <c r="PNV3" s="1"/>
+      <c r="POD3" s="1"/>
+      <c r="POL3" s="1"/>
+      <c r="POT3" s="1"/>
+      <c r="PPB3" s="1"/>
+      <c r="PPJ3" s="1"/>
+      <c r="PPR3" s="1"/>
+      <c r="PPZ3" s="1"/>
+      <c r="PQH3" s="1"/>
+      <c r="PQP3" s="1"/>
+      <c r="PQX3" s="1"/>
+      <c r="PRF3" s="1"/>
+      <c r="PRN3" s="1"/>
+      <c r="PRV3" s="1"/>
+      <c r="PSD3" s="1"/>
+      <c r="PSL3" s="1"/>
+      <c r="PST3" s="1"/>
+      <c r="PTB3" s="1"/>
+      <c r="PTJ3" s="1"/>
+      <c r="PTR3" s="1"/>
+      <c r="PTZ3" s="1"/>
+      <c r="PUH3" s="1"/>
+      <c r="PUP3" s="1"/>
+      <c r="PUX3" s="1"/>
+      <c r="PVF3" s="1"/>
+      <c r="PVN3" s="1"/>
+      <c r="PVV3" s="1"/>
+      <c r="PWD3" s="1"/>
+      <c r="PWL3" s="1"/>
+      <c r="PWT3" s="1"/>
+      <c r="PXB3" s="1"/>
+      <c r="PXJ3" s="1"/>
+      <c r="PXR3" s="1"/>
+      <c r="PXZ3" s="1"/>
+      <c r="PYH3" s="1"/>
+      <c r="PYP3" s="1"/>
+      <c r="PYX3" s="1"/>
+      <c r="PZF3" s="1"/>
+      <c r="PZN3" s="1"/>
+      <c r="PZV3" s="1"/>
+      <c r="QAD3" s="1"/>
+      <c r="QAL3" s="1"/>
+      <c r="QAT3" s="1"/>
+      <c r="QBB3" s="1"/>
+      <c r="QBJ3" s="1"/>
+      <c r="QBR3" s="1"/>
+      <c r="QBZ3" s="1"/>
+      <c r="QCH3" s="1"/>
+      <c r="QCP3" s="1"/>
+      <c r="QCX3" s="1"/>
+      <c r="QDF3" s="1"/>
+      <c r="QDN3" s="1"/>
+      <c r="QDV3" s="1"/>
+      <c r="QED3" s="1"/>
+      <c r="QEL3" s="1"/>
+      <c r="QET3" s="1"/>
+      <c r="QFB3" s="1"/>
+      <c r="QFJ3" s="1"/>
+      <c r="QFR3" s="1"/>
+      <c r="QFZ3" s="1"/>
+      <c r="QGH3" s="1"/>
+      <c r="QGP3" s="1"/>
+      <c r="QGX3" s="1"/>
+      <c r="QHF3" s="1"/>
+      <c r="QHN3" s="1"/>
+      <c r="QHV3" s="1"/>
+      <c r="QID3" s="1"/>
+      <c r="QIL3" s="1"/>
+      <c r="QIT3" s="1"/>
+      <c r="QJB3" s="1"/>
+      <c r="QJJ3" s="1"/>
+      <c r="QJR3" s="1"/>
+      <c r="QJZ3" s="1"/>
+      <c r="QKH3" s="1"/>
+      <c r="QKP3" s="1"/>
+      <c r="QKX3" s="1"/>
+      <c r="QLF3" s="1"/>
+      <c r="QLN3" s="1"/>
+      <c r="QLV3" s="1"/>
+      <c r="QMD3" s="1"/>
+      <c r="QML3" s="1"/>
+      <c r="QMT3" s="1"/>
+      <c r="QNB3" s="1"/>
+      <c r="QNJ3" s="1"/>
+      <c r="QNR3" s="1"/>
+      <c r="QNZ3" s="1"/>
+      <c r="QOH3" s="1"/>
+      <c r="QOP3" s="1"/>
+      <c r="QOX3" s="1"/>
+      <c r="QPF3" s="1"/>
+      <c r="QPN3" s="1"/>
+      <c r="QPV3" s="1"/>
+      <c r="QQD3" s="1"/>
+      <c r="QQL3" s="1"/>
+      <c r="QQT3" s="1"/>
+      <c r="QRB3" s="1"/>
+      <c r="QRJ3" s="1"/>
+      <c r="QRR3" s="1"/>
+      <c r="QRZ3" s="1"/>
+      <c r="QSH3" s="1"/>
+      <c r="QSP3" s="1"/>
+      <c r="QSX3" s="1"/>
+      <c r="QTF3" s="1"/>
+      <c r="QTN3" s="1"/>
+      <c r="QTV3" s="1"/>
+      <c r="QUD3" s="1"/>
+      <c r="QUL3" s="1"/>
+      <c r="QUT3" s="1"/>
+      <c r="QVB3" s="1"/>
+      <c r="QVJ3" s="1"/>
+      <c r="QVR3" s="1"/>
+      <c r="QVZ3" s="1"/>
+      <c r="QWH3" s="1"/>
+      <c r="QWP3" s="1"/>
+      <c r="QWX3" s="1"/>
+      <c r="QXF3" s="1"/>
+      <c r="QXN3" s="1"/>
+      <c r="QXV3" s="1"/>
+      <c r="QYD3" s="1"/>
+      <c r="QYL3" s="1"/>
+      <c r="QYT3" s="1"/>
+      <c r="QZB3" s="1"/>
+      <c r="QZJ3" s="1"/>
+      <c r="QZR3" s="1"/>
+      <c r="QZZ3" s="1"/>
+      <c r="RAH3" s="1"/>
+      <c r="RAP3" s="1"/>
+      <c r="RAX3" s="1"/>
+      <c r="RBF3" s="1"/>
+      <c r="RBN3" s="1"/>
+      <c r="RBV3" s="1"/>
+      <c r="RCD3" s="1"/>
+      <c r="RCL3" s="1"/>
+      <c r="RCT3" s="1"/>
+      <c r="RDB3" s="1"/>
+      <c r="RDJ3" s="1"/>
+      <c r="RDR3" s="1"/>
+      <c r="RDZ3" s="1"/>
+      <c r="REH3" s="1"/>
+      <c r="REP3" s="1"/>
+      <c r="REX3" s="1"/>
+      <c r="RFF3" s="1"/>
+      <c r="RFN3" s="1"/>
+      <c r="RFV3" s="1"/>
+      <c r="RGD3" s="1"/>
+      <c r="RGL3" s="1"/>
+      <c r="RGT3" s="1"/>
+      <c r="RHB3" s="1"/>
+      <c r="RHJ3" s="1"/>
+      <c r="RHR3" s="1"/>
+      <c r="RHZ3" s="1"/>
+      <c r="RIH3" s="1"/>
+      <c r="RIP3" s="1"/>
+      <c r="RIX3" s="1"/>
+      <c r="RJF3" s="1"/>
+      <c r="RJN3" s="1"/>
+      <c r="RJV3" s="1"/>
+      <c r="RKD3" s="1"/>
+      <c r="RKL3" s="1"/>
+      <c r="RKT3" s="1"/>
+      <c r="RLB3" s="1"/>
+      <c r="RLJ3" s="1"/>
+      <c r="RLR3" s="1"/>
+      <c r="RLZ3" s="1"/>
+      <c r="RMH3" s="1"/>
+      <c r="RMP3" s="1"/>
+      <c r="RMX3" s="1"/>
+      <c r="RNF3" s="1"/>
+      <c r="RNN3" s="1"/>
+      <c r="RNV3" s="1"/>
+      <c r="ROD3" s="1"/>
+      <c r="ROL3" s="1"/>
+      <c r="ROT3" s="1"/>
+      <c r="RPB3" s="1"/>
+      <c r="RPJ3" s="1"/>
+      <c r="RPR3" s="1"/>
+      <c r="RPZ3" s="1"/>
+      <c r="RQH3" s="1"/>
+      <c r="RQP3" s="1"/>
+      <c r="RQX3" s="1"/>
+      <c r="RRF3" s="1"/>
+      <c r="RRN3" s="1"/>
+      <c r="RRV3" s="1"/>
+      <c r="RSD3" s="1"/>
+      <c r="RSL3" s="1"/>
+      <c r="RST3" s="1"/>
+      <c r="RTB3" s="1"/>
+      <c r="RTJ3" s="1"/>
+      <c r="RTR3" s="1"/>
+      <c r="RTZ3" s="1"/>
+      <c r="RUH3" s="1"/>
+      <c r="RUP3" s="1"/>
+      <c r="RUX3" s="1"/>
+      <c r="RVF3" s="1"/>
+      <c r="RVN3" s="1"/>
+      <c r="RVV3" s="1"/>
+      <c r="RWD3" s="1"/>
+      <c r="RWL3" s="1"/>
+      <c r="RWT3" s="1"/>
+      <c r="RXB3" s="1"/>
+      <c r="RXJ3" s="1"/>
+      <c r="RXR3" s="1"/>
+      <c r="RXZ3" s="1"/>
+      <c r="RYH3" s="1"/>
+      <c r="RYP3" s="1"/>
+      <c r="RYX3" s="1"/>
+      <c r="RZF3" s="1"/>
+      <c r="RZN3" s="1"/>
+      <c r="RZV3" s="1"/>
+      <c r="SAD3" s="1"/>
+      <c r="SAL3" s="1"/>
+      <c r="SAT3" s="1"/>
+      <c r="SBB3" s="1"/>
+      <c r="SBJ3" s="1"/>
+      <c r="SBR3" s="1"/>
+      <c r="SBZ3" s="1"/>
+      <c r="SCH3" s="1"/>
+      <c r="SCP3" s="1"/>
+      <c r="SCX3" s="1"/>
+      <c r="SDF3" s="1"/>
+      <c r="SDN3" s="1"/>
+      <c r="SDV3" s="1"/>
+      <c r="SED3" s="1"/>
+      <c r="SEL3" s="1"/>
+      <c r="SET3" s="1"/>
+      <c r="SFB3" s="1"/>
+      <c r="SFJ3" s="1"/>
+      <c r="SFR3" s="1"/>
+      <c r="SFZ3" s="1"/>
+      <c r="SGH3" s="1"/>
+      <c r="SGP3" s="1"/>
+      <c r="SGX3" s="1"/>
+      <c r="SHF3" s="1"/>
+      <c r="SHN3" s="1"/>
+      <c r="SHV3" s="1"/>
+      <c r="SID3" s="1"/>
+      <c r="SIL3" s="1"/>
+      <c r="SIT3" s="1"/>
+      <c r="SJB3" s="1"/>
+      <c r="SJJ3" s="1"/>
+      <c r="SJR3" s="1"/>
+      <c r="SJZ3" s="1"/>
+      <c r="SKH3" s="1"/>
+      <c r="SKP3" s="1"/>
+      <c r="SKX3" s="1"/>
+      <c r="SLF3" s="1"/>
+      <c r="SLN3" s="1"/>
+      <c r="SLV3" s="1"/>
+      <c r="SMD3" s="1"/>
+      <c r="SML3" s="1"/>
+      <c r="SMT3" s="1"/>
+      <c r="SNB3" s="1"/>
+      <c r="SNJ3" s="1"/>
+      <c r="SNR3" s="1"/>
+      <c r="SNZ3" s="1"/>
+      <c r="SOH3" s="1"/>
+      <c r="SOP3" s="1"/>
+      <c r="SOX3" s="1"/>
+      <c r="SPF3" s="1"/>
+      <c r="SPN3" s="1"/>
+      <c r="SPV3" s="1"/>
+      <c r="SQD3" s="1"/>
+      <c r="SQL3" s="1"/>
+      <c r="SQT3" s="1"/>
+      <c r="SRB3" s="1"/>
+      <c r="SRJ3" s="1"/>
+      <c r="SRR3" s="1"/>
+      <c r="SRZ3" s="1"/>
+      <c r="SSH3" s="1"/>
+      <c r="SSP3" s="1"/>
+      <c r="SSX3" s="1"/>
+      <c r="STF3" s="1"/>
+      <c r="STN3" s="1"/>
+      <c r="STV3" s="1"/>
+      <c r="SUD3" s="1"/>
+      <c r="SUL3" s="1"/>
+      <c r="SUT3" s="1"/>
+      <c r="SVB3" s="1"/>
+      <c r="SVJ3" s="1"/>
+      <c r="SVR3" s="1"/>
+      <c r="SVZ3" s="1"/>
+      <c r="SWH3" s="1"/>
+      <c r="SWP3" s="1"/>
+      <c r="SWX3" s="1"/>
+      <c r="SXF3" s="1"/>
+      <c r="SXN3" s="1"/>
+      <c r="SXV3" s="1"/>
+      <c r="SYD3" s="1"/>
+      <c r="SYL3" s="1"/>
+      <c r="SYT3" s="1"/>
+      <c r="SZB3" s="1"/>
+      <c r="SZJ3" s="1"/>
+      <c r="SZR3" s="1"/>
+      <c r="SZZ3" s="1"/>
+      <c r="TAH3" s="1"/>
+      <c r="TAP3" s="1"/>
+      <c r="TAX3" s="1"/>
+      <c r="TBF3" s="1"/>
+      <c r="TBN3" s="1"/>
+      <c r="TBV3" s="1"/>
+      <c r="TCD3" s="1"/>
+      <c r="TCL3" s="1"/>
+      <c r="TCT3" s="1"/>
+      <c r="TDB3" s="1"/>
+      <c r="TDJ3" s="1"/>
+      <c r="TDR3" s="1"/>
+      <c r="TDZ3" s="1"/>
+      <c r="TEH3" s="1"/>
+      <c r="TEP3" s="1"/>
+      <c r="TEX3" s="1"/>
+      <c r="TFF3" s="1"/>
+      <c r="TFN3" s="1"/>
+      <c r="TFV3" s="1"/>
+      <c r="TGD3" s="1"/>
+      <c r="TGL3" s="1"/>
+      <c r="TGT3" s="1"/>
+      <c r="THB3" s="1"/>
+      <c r="THJ3" s="1"/>
+      <c r="THR3" s="1"/>
+      <c r="THZ3" s="1"/>
+      <c r="TIH3" s="1"/>
+      <c r="TIP3" s="1"/>
+      <c r="TIX3" s="1"/>
+      <c r="TJF3" s="1"/>
+      <c r="TJN3" s="1"/>
+      <c r="TJV3" s="1"/>
+      <c r="TKD3" s="1"/>
+      <c r="TKL3" s="1"/>
+      <c r="TKT3" s="1"/>
+      <c r="TLB3" s="1"/>
+      <c r="TLJ3" s="1"/>
+      <c r="TLR3" s="1"/>
+      <c r="TLZ3" s="1"/>
+      <c r="TMH3" s="1"/>
+      <c r="TMP3" s="1"/>
+      <c r="TMX3" s="1"/>
+      <c r="TNF3" s="1"/>
+      <c r="TNN3" s="1"/>
+      <c r="TNV3" s="1"/>
+      <c r="TOD3" s="1"/>
+      <c r="TOL3" s="1"/>
+      <c r="TOT3" s="1"/>
+      <c r="TPB3" s="1"/>
+      <c r="TPJ3" s="1"/>
+      <c r="TPR3" s="1"/>
+      <c r="TPZ3" s="1"/>
+      <c r="TQH3" s="1"/>
+      <c r="TQP3" s="1"/>
+      <c r="TQX3" s="1"/>
+      <c r="TRF3" s="1"/>
+      <c r="TRN3" s="1"/>
+      <c r="TRV3" s="1"/>
+      <c r="TSD3" s="1"/>
+      <c r="TSL3" s="1"/>
+      <c r="TST3" s="1"/>
+      <c r="TTB3" s="1"/>
+      <c r="TTJ3" s="1"/>
+      <c r="TTR3" s="1"/>
+      <c r="TTZ3" s="1"/>
+      <c r="TUH3" s="1"/>
+      <c r="TUP3" s="1"/>
+      <c r="TUX3" s="1"/>
+      <c r="TVF3" s="1"/>
+      <c r="TVN3" s="1"/>
+      <c r="TVV3" s="1"/>
+      <c r="TWD3" s="1"/>
+      <c r="TWL3" s="1"/>
+      <c r="TWT3" s="1"/>
+      <c r="TXB3" s="1"/>
+      <c r="TXJ3" s="1"/>
+      <c r="TXR3" s="1"/>
+      <c r="TXZ3" s="1"/>
+      <c r="TYH3" s="1"/>
+      <c r="TYP3" s="1"/>
+      <c r="TYX3" s="1"/>
+      <c r="TZF3" s="1"/>
+      <c r="TZN3" s="1"/>
+      <c r="TZV3" s="1"/>
+      <c r="UAD3" s="1"/>
+      <c r="UAL3" s="1"/>
+      <c r="UAT3" s="1"/>
+      <c r="UBB3" s="1"/>
+      <c r="UBJ3" s="1"/>
+      <c r="UBR3" s="1"/>
+      <c r="UBZ3" s="1"/>
+      <c r="UCH3" s="1"/>
+      <c r="UCP3" s="1"/>
+      <c r="UCX3" s="1"/>
+      <c r="UDF3" s="1"/>
+      <c r="UDN3" s="1"/>
+      <c r="UDV3" s="1"/>
+      <c r="UED3" s="1"/>
+      <c r="UEL3" s="1"/>
+      <c r="UET3" s="1"/>
+      <c r="UFB3" s="1"/>
+      <c r="UFJ3" s="1"/>
+      <c r="UFR3" s="1"/>
+      <c r="UFZ3" s="1"/>
+      <c r="UGH3" s="1"/>
+      <c r="UGP3" s="1"/>
+      <c r="UGX3" s="1"/>
+      <c r="UHF3" s="1"/>
+      <c r="UHN3" s="1"/>
+      <c r="UHV3" s="1"/>
+      <c r="UID3" s="1"/>
+      <c r="UIL3" s="1"/>
+      <c r="UIT3" s="1"/>
+      <c r="UJB3" s="1"/>
+      <c r="UJJ3" s="1"/>
+      <c r="UJR3" s="1"/>
+      <c r="UJZ3" s="1"/>
+      <c r="UKH3" s="1"/>
+      <c r="UKP3" s="1"/>
+      <c r="UKX3" s="1"/>
+      <c r="ULF3" s="1"/>
+      <c r="ULN3" s="1"/>
+      <c r="ULV3" s="1"/>
+      <c r="UMD3" s="1"/>
+      <c r="UML3" s="1"/>
+      <c r="UMT3" s="1"/>
+      <c r="UNB3" s="1"/>
+      <c r="UNJ3" s="1"/>
+      <c r="UNR3" s="1"/>
+      <c r="UNZ3" s="1"/>
+      <c r="UOH3" s="1"/>
+      <c r="UOP3" s="1"/>
+      <c r="UOX3" s="1"/>
+      <c r="UPF3" s="1"/>
+      <c r="UPN3" s="1"/>
+      <c r="UPV3" s="1"/>
+      <c r="UQD3" s="1"/>
+      <c r="UQL3" s="1"/>
+      <c r="UQT3" s="1"/>
+      <c r="URB3" s="1"/>
+      <c r="URJ3" s="1"/>
+      <c r="URR3" s="1"/>
+      <c r="URZ3" s="1"/>
+      <c r="USH3" s="1"/>
+      <c r="USP3" s="1"/>
+      <c r="USX3" s="1"/>
+      <c r="UTF3" s="1"/>
+      <c r="UTN3" s="1"/>
+      <c r="UTV3" s="1"/>
+      <c r="UUD3" s="1"/>
+      <c r="UUL3" s="1"/>
+      <c r="UUT3" s="1"/>
+      <c r="UVB3" s="1"/>
+      <c r="UVJ3" s="1"/>
+      <c r="UVR3" s="1"/>
+      <c r="UVZ3" s="1"/>
+      <c r="UWH3" s="1"/>
+      <c r="UWP3" s="1"/>
+      <c r="UWX3" s="1"/>
+      <c r="UXF3" s="1"/>
+      <c r="UXN3" s="1"/>
+      <c r="UXV3" s="1"/>
+      <c r="UYD3" s="1"/>
+      <c r="UYL3" s="1"/>
+      <c r="UYT3" s="1"/>
+      <c r="UZB3" s="1"/>
+      <c r="UZJ3" s="1"/>
+      <c r="UZR3" s="1"/>
+      <c r="UZZ3" s="1"/>
+      <c r="VAH3" s="1"/>
+      <c r="VAP3" s="1"/>
+      <c r="VAX3" s="1"/>
+      <c r="VBF3" s="1"/>
+      <c r="VBN3" s="1"/>
+      <c r="VBV3" s="1"/>
+      <c r="VCD3" s="1"/>
+      <c r="VCL3" s="1"/>
+      <c r="VCT3" s="1"/>
+      <c r="VDB3" s="1"/>
+      <c r="VDJ3" s="1"/>
+      <c r="VDR3" s="1"/>
+      <c r="VDZ3" s="1"/>
+      <c r="VEH3" s="1"/>
+      <c r="VEP3" s="1"/>
+      <c r="VEX3" s="1"/>
+      <c r="VFF3" s="1"/>
+      <c r="VFN3" s="1"/>
+      <c r="VFV3" s="1"/>
+      <c r="VGD3" s="1"/>
+      <c r="VGL3" s="1"/>
+      <c r="VGT3" s="1"/>
+      <c r="VHB3" s="1"/>
+      <c r="VHJ3" s="1"/>
+      <c r="VHR3" s="1"/>
+      <c r="VHZ3" s="1"/>
+      <c r="VIH3" s="1"/>
+      <c r="VIP3" s="1"/>
+      <c r="VIX3" s="1"/>
+      <c r="VJF3" s="1"/>
+      <c r="VJN3" s="1"/>
+      <c r="VJV3" s="1"/>
+      <c r="VKD3" s="1"/>
+      <c r="VKL3" s="1"/>
+      <c r="VKT3" s="1"/>
+      <c r="VLB3" s="1"/>
+      <c r="VLJ3" s="1"/>
+      <c r="VLR3" s="1"/>
+      <c r="VLZ3" s="1"/>
+      <c r="VMH3" s="1"/>
+      <c r="VMP3" s="1"/>
+      <c r="VMX3" s="1"/>
+      <c r="VNF3" s="1"/>
+      <c r="VNN3" s="1"/>
+      <c r="VNV3" s="1"/>
+      <c r="VOD3" s="1"/>
+      <c r="VOL3" s="1"/>
+      <c r="VOT3" s="1"/>
+      <c r="VPB3" s="1"/>
+      <c r="VPJ3" s="1"/>
+      <c r="VPR3" s="1"/>
+      <c r="VPZ3" s="1"/>
+      <c r="VQH3" s="1"/>
+      <c r="VQP3" s="1"/>
+      <c r="VQX3" s="1"/>
+      <c r="VRF3" s="1"/>
+      <c r="VRN3" s="1"/>
+      <c r="VRV3" s="1"/>
+      <c r="VSD3" s="1"/>
+      <c r="VSL3" s="1"/>
+      <c r="VST3" s="1"/>
+      <c r="VTB3" s="1"/>
+      <c r="VTJ3" s="1"/>
+      <c r="VTR3" s="1"/>
+      <c r="VTZ3" s="1"/>
+      <c r="VUH3" s="1"/>
+      <c r="VUP3" s="1"/>
+      <c r="VUX3" s="1"/>
+      <c r="VVF3" s="1"/>
+      <c r="VVN3" s="1"/>
+      <c r="VVV3" s="1"/>
+      <c r="VWD3" s="1"/>
+      <c r="VWL3" s="1"/>
+      <c r="VWT3" s="1"/>
+      <c r="VXB3" s="1"/>
+      <c r="VXJ3" s="1"/>
+      <c r="VXR3" s="1"/>
+      <c r="VXZ3" s="1"/>
+      <c r="VYH3" s="1"/>
+      <c r="VYP3" s="1"/>
+      <c r="VYX3" s="1"/>
+      <c r="VZF3" s="1"/>
+      <c r="VZN3" s="1"/>
+      <c r="VZV3" s="1"/>
+      <c r="WAD3" s="1"/>
+      <c r="WAL3" s="1"/>
+      <c r="WAT3" s="1"/>
+      <c r="WBB3" s="1"/>
+      <c r="WBJ3" s="1"/>
+      <c r="WBR3" s="1"/>
+      <c r="WBZ3" s="1"/>
+      <c r="WCH3" s="1"/>
+      <c r="WCP3" s="1"/>
+      <c r="WCX3" s="1"/>
+      <c r="WDF3" s="1"/>
+      <c r="WDN3" s="1"/>
+      <c r="WDV3" s="1"/>
+      <c r="WED3" s="1"/>
+      <c r="WEL3" s="1"/>
+      <c r="WET3" s="1"/>
+      <c r="WFB3" s="1"/>
+      <c r="WFJ3" s="1"/>
+      <c r="WFR3" s="1"/>
+      <c r="WFZ3" s="1"/>
+      <c r="WGH3" s="1"/>
+      <c r="WGP3" s="1"/>
+      <c r="WGX3" s="1"/>
+      <c r="WHF3" s="1"/>
+      <c r="WHN3" s="1"/>
+      <c r="WHV3" s="1"/>
+      <c r="WID3" s="1"/>
+      <c r="WIL3" s="1"/>
+      <c r="WIT3" s="1"/>
+      <c r="WJB3" s="1"/>
+      <c r="WJJ3" s="1"/>
+      <c r="WJR3" s="1"/>
+      <c r="WJZ3" s="1"/>
+      <c r="WKH3" s="1"/>
+      <c r="WKP3" s="1"/>
+      <c r="WKX3" s="1"/>
+      <c r="WLF3" s="1"/>
+      <c r="WLN3" s="1"/>
+      <c r="WLV3" s="1"/>
+      <c r="WMD3" s="1"/>
+      <c r="WML3" s="1"/>
+      <c r="WMT3" s="1"/>
+      <c r="WNB3" s="1"/>
+      <c r="WNJ3" s="1"/>
+      <c r="WNR3" s="1"/>
+      <c r="WNZ3" s="1"/>
+      <c r="WOH3" s="1"/>
+      <c r="WOP3" s="1"/>
+      <c r="WOX3" s="1"/>
+      <c r="WPF3" s="1"/>
+      <c r="WPN3" s="1"/>
+      <c r="WPV3" s="1"/>
+      <c r="WQD3" s="1"/>
+      <c r="WQL3" s="1"/>
+      <c r="WQT3" s="1"/>
+      <c r="WRB3" s="1"/>
+      <c r="WRJ3" s="1"/>
+      <c r="WRR3" s="1"/>
+      <c r="WRZ3" s="1"/>
+      <c r="WSH3" s="1"/>
+      <c r="WSP3" s="1"/>
+      <c r="WSX3" s="1"/>
+      <c r="WTF3" s="1"/>
+      <c r="WTN3" s="1"/>
+      <c r="WTV3" s="1"/>
+      <c r="WUD3" s="1"/>
+      <c r="WUL3" s="1"/>
+      <c r="WUT3" s="1"/>
+      <c r="WVB3" s="1"/>
+      <c r="WVJ3" s="1"/>
+      <c r="WVR3" s="1"/>
+      <c r="WVZ3" s="1"/>
+      <c r="WWH3" s="1"/>
+      <c r="WWP3" s="1"/>
+      <c r="WWX3" s="1"/>
+      <c r="WXF3" s="1"/>
+      <c r="WXN3" s="1"/>
+      <c r="WXV3" s="1"/>
+      <c r="WYD3" s="1"/>
+      <c r="WYL3" s="1"/>
+      <c r="WYT3" s="1"/>
+      <c r="WZB3" s="1"/>
+      <c r="WZJ3" s="1"/>
+      <c r="WZR3" s="1"/>
+      <c r="WZZ3" s="1"/>
+      <c r="XAH3" s="1"/>
+      <c r="XAP3" s="1"/>
+      <c r="XAX3" s="1"/>
+      <c r="XBF3" s="1"/>
+      <c r="XBN3" s="1"/>
+      <c r="XBV3" s="1"/>
+      <c r="XCD3" s="1"/>
+      <c r="XCL3" s="1"/>
+      <c r="XCT3" s="1"/>
+      <c r="XDB3" s="1"/>
+      <c r="XDJ3" s="1"/>
+      <c r="XDR3" s="1"/>
+      <c r="XDZ3" s="1"/>
+      <c r="XEH3" s="1"/>
+      <c r="XEP3" s="1"/>
+      <c r="XEX3" s="1"/>
+    </row>
+    <row r="4" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B4" s="7">
         <v>4.8210000000000001E-4</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C4" s="5">
         <v>4.1000000000000003E-3</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D4" s="7">
         <v>-4.728E-7</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E4" s="6">
         <v>0.137267</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="6">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="6">
         <v>0.48180000000000001</v>
       </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="6">
+        <v>-61.598500000000001</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="H5" s="6">
+        <v>5.398E-2</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="6">
-        <v>-61.598500000000001</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="H4" s="6">
-        <v>5.398E-2</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="7">
+      <c r="B6" s="7">
         <v>6.4670000000000005E-4</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C6" s="5">
         <v>8.8199999999999997E-3</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D6" s="7">
         <v>-2.9900000000000002E-7</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E6" s="6">
         <v>0.34514</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F6" s="7">
         <v>138.5</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G6" s="6">
         <v>0.16696</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H6" s="6">
         <v>0.48859999999999998</v>
       </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="7">
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="7">
         <v>4.1839999999999998E-4</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C7" s="15">
         <v>1.1900000000000001E-2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D7" s="7">
         <v>-4.0649999999999999E-7</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E7" s="6">
         <v>0.21010000000000001</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="6">
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="6">
         <v>0.39639999999999997</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="8" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="7">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="7">
         <v>46.827800000000003</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G8" s="6">
         <v>0.39700000000000002</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H8" s="6">
         <v>5.1679999999999997E-2</v>
       </c>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B9" s="13">
         <v>3.1690000000000001E-4</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C9" s="5">
         <v>3.1600000000000003E-2</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D9" s="13">
         <v>-4.5429999999999999E-7</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E9" s="6">
         <v>0.19550000000000001</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="6">
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="6">
         <v>0.25590000000000002</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I9" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1150,8 +3219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC43E702-708E-4929-83A6-563C048BC86A}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1978,7 +4047,7 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:I7"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Clean and organize files before archiving
</commit_message>
<xml_diff>
--- a/data/ModelResults.xlsx
+++ b/data/ModelResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/connerj_msu_edu/Documents/DocumentsOneDrive/Files/ConnerLabOneDrive/Arabidopsis/Stamen loss/European Population Surveys/Pyrenees/SophieAnalyses/R_script/StamenLossPipeline/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="393" documentId="8_{A5E90707-7E9A-4109-AE1B-D5AE205301FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{896A7CE6-D3FE-4874-9AC1-0D3E3ED368BD}"/>
+  <xr:revisionPtr revIDLastSave="394" documentId="8_{A5E90707-7E9A-4109-AE1B-D5AE205301FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{984D82AC-BA46-457C-94D0-FC573B22C95C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6D0F4C7-BFDF-463E-8B4C-67AB0A4A9DEB}"/>
+    <workbookView minimized="1" xWindow="345" yWindow="2475" windowWidth="7425" windowHeight="4740" xr2:uid="{E6D0F4C7-BFDF-463E-8B4C-67AB0A4A9DEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Formatted" sheetId="3" r:id="rId1"/>
@@ -320,32 +320,6 @@
     <t>Seq_PopFlwrMean ~ Nucleotide Diversity</t>
   </si>
   <si>
-    <r>
-      <t>Seq_PopFlwrMean ~ Elevation + (centered Elevation)</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> + Nucldotide Diversity</t>
-    </r>
-  </si>
-  <si>
     <t>Elevation estimate</t>
   </si>
   <si>
@@ -430,6 +404,32 @@
   </si>
   <si>
     <t>Elevation is linear here</t>
+  </si>
+  <si>
+    <r>
+      <t>Seq_PopFlwrMean ~ Elevation + (centered Elevation)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + Nucleotide Diversity</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -621,9 +621,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -661,7 +661,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -767,7 +767,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -909,7 +909,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -944,7 +944,7 @@
   <dimension ref="A1:XEX9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,22 +980,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>15</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="3" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="7">
         <v>-1.8059999999999999E-6</v>
@@ -1022,7 +1022,7 @@
         <v>0.6411</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J3" s="1"/>
       <c r="R3" s="1"/>
@@ -3118,7 +3118,7 @@
     </row>
     <row r="6" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B6" s="7">
         <v>6.4670000000000005E-4</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="7" spans="1:1018 1026:2042 2050:3066 3074:4090 4098:5114 5122:6138 6146:7162 7170:8186 8194:9210 9218:10234 10242:11258 11266:12282 12290:13306 13314:14330 14338:15354 15362:16378" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="7">
         <v>4.1839999999999998E-4</v>

</xml_diff>